<commit_message>
Added BK 25m1pijl teams
</commit_message>
<xml_diff>
--- a/CompLaagBond/files/template-excel-bk-25m1pijl-indiv.xlsx
+++ b/CompLaagBond/files/template-excel-bk-25m1pijl-indiv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects Ramon\Websites\NHB-applicaties\Excel programma's\BK excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD29EFD-B874-4371-BD12-C4DD3BDE46F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4765E9F9-53EE-422A-8CE0-849CEE970DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5265" yWindow="1035" windowWidth="22440" windowHeight="14040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="75" yWindow="1425" windowWidth="22440" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Uitleg (2)" sheetId="5" r:id="rId1"/>
@@ -782,52 +782,52 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
+      <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1193,9 +1193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A6380CA-469D-4A31-B933-BC719C1B440A}">
   <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1588,9 +1586,7 @@
   </sheetPr>
   <dimension ref="A1:Y250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1640,25 +1636,25 @@
       <c r="U1" s="3"/>
     </row>
     <row r="2" spans="1:25" ht="18" x14ac:dyDescent="0.25">
-      <c r="C2" s="74" t="str">
+      <c r="C2" s="76" t="str">
         <f>"Bondskampioenschappen 25m1pijl &lt;seizoen&gt;, &lt;klasse&gt;"</f>
         <v>Bondskampioenschappen 25m1pijl &lt;seizoen&gt;, &lt;klasse&gt;</v>
       </c>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="75"/>
-      <c r="O2" s="75"/>
-      <c r="P2" s="75"/>
-      <c r="Q2" s="75"/>
-      <c r="R2" s="76"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
+      <c r="N2" s="77"/>
+      <c r="O2" s="77"/>
+      <c r="P2" s="77"/>
+      <c r="Q2" s="77"/>
+      <c r="R2" s="78"/>
       <c r="T2" s="21" t="s">
         <v>60</v>
       </c>
@@ -1666,34 +1662,34 @@
     </row>
     <row r="3" spans="1:25" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="55"/>
-      <c r="D3" s="72" t="s">
+      <c r="D3" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="72"/>
+      <c r="E3" s="74"/>
       <c r="F3" s="50"/>
       <c r="G3" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="79" t="s">
+      <c r="H3" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="79"/>
+      <c r="I3" s="81"/>
       <c r="J3" s="68"/>
       <c r="K3" s="54"/>
       <c r="L3" s="54"/>
-      <c r="M3" s="72" t="s">
+      <c r="M3" s="74" t="s">
         <v>73</v>
       </c>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="72"/>
-      <c r="Q3" s="72"/>
-      <c r="R3" s="73"/>
-      <c r="S3" s="82" t="s">
+      <c r="N3" s="74"/>
+      <c r="O3" s="74"/>
+      <c r="P3" s="74"/>
+      <c r="Q3" s="74"/>
+      <c r="R3" s="75"/>
+      <c r="S3" s="71" t="s">
         <v>59</v>
       </c>
-      <c r="T3" s="81"/>
-      <c r="U3" s="81"/>
+      <c r="T3" s="72"/>
+      <c r="U3" s="72"/>
     </row>
     <row r="4" spans="1:25" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C4" s="55"/>
@@ -1703,15 +1699,15 @@
       <c r="G4" s="51"/>
       <c r="H4" s="52"/>
       <c r="I4" s="52"/>
-      <c r="J4" s="80" t="s">
+      <c r="J4" s="82" t="s">
         <v>52</v>
       </c>
-      <c r="K4" s="80"/>
+      <c r="K4" s="82"/>
       <c r="L4" s="54"/>
-      <c r="M4" s="77" t="s">
+      <c r="M4" s="79" t="s">
         <v>62</v>
       </c>
-      <c r="N4" s="77"/>
+      <c r="N4" s="79"/>
       <c r="O4" s="25"/>
       <c r="P4" s="53"/>
       <c r="Q4" s="53"/>
@@ -1730,10 +1726,10 @@
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="78"/>
+      <c r="B5" s="80"/>
       <c r="C5" s="56">
         <v>0</v>
       </c>
@@ -2722,16 +2718,16 @@
       <c r="I33" s="12"/>
       <c r="J33" s="24"/>
       <c r="K33" s="24"/>
-      <c r="L33" s="71" t="s">
+      <c r="L33" s="73" t="s">
         <v>58</v>
       </c>
-      <c r="M33" s="71"/>
-      <c r="N33" s="71"/>
-      <c r="O33" s="71"/>
-      <c r="P33" s="71"/>
-      <c r="Q33" s="71"/>
-      <c r="R33" s="71"/>
-      <c r="S33" s="71"/>
+      <c r="M33" s="73"/>
+      <c r="N33" s="73"/>
+      <c r="O33" s="73"/>
+      <c r="P33" s="73"/>
+      <c r="Q33" s="73"/>
+      <c r="R33" s="73"/>
+      <c r="S33" s="73"/>
       <c r="T33" s="44"/>
       <c r="U33" s="44"/>
       <c r="V33"/>
@@ -2982,15 +2978,15 @@
     <sortCondition descending="1" ref="S6:S29"/>
   </sortState>
   <mergeCells count="9">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J4:K4"/>
     <mergeCell ref="S3:U3"/>
     <mergeCell ref="L33:S33"/>
     <mergeCell ref="M3:R3"/>
     <mergeCell ref="C2:R2"/>
     <mergeCell ref="M4:N4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="S6:S29">

</xml_diff>

<commit_message>
Swap column headers on page Uitslag
</commit_message>
<xml_diff>
--- a/CompLaagBond/files/template-excel-bk-25m1pijl-indiv.xlsx
+++ b/CompLaagBond/files/template-excel-bk-25m1pijl-indiv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects Ramon\Websites\NHB-applicaties\Excel programma's\BK excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E38CFD0-57FB-41DA-9CA1-99D1612F707E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD0EE06-F202-41CC-882B-D2BA9CB0DBAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="1290" windowWidth="22440" windowHeight="14040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3615" yWindow="720" windowWidth="22440" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Uitleg" sheetId="5" r:id="rId1"/>
@@ -741,7 +741,7 @@
     <cellStyle name="Normal 2" xfId="2" xr:uid="{C91EDC24-51C3-4FC0-9914-71A273B5E286}"/>
     <cellStyle name="Standaard_Vers" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -755,32 +755,11 @@
     <dxf>
       <font>
         <strike val="0"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
         <color auto="1"/>
       </font>
       <fill>
         <patternFill patternType="solid">
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1120,7 +1099,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A6380CA-469D-4A31-B933-BC719C1B440A}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1361,7 +1340,7 @@
   </sheetPr>
   <dimension ref="A3:Y252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -2780,10 +2759,10 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="S8:S31">
-    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.35433070866141736" right="0.39370078740157483" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" scale="89" fitToHeight="10" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Corrected description phase N
</commit_message>
<xml_diff>
--- a/CompLaagBond/files/template-excel-bk-25m1pijl-indiv.xlsx
+++ b/CompLaagBond/files/template-excel-bk-25m1pijl-indiv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects Ramon\Websites\NHB-applicaties\Excel programma's\BK excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD0EE06-F202-41CC-882B-D2BA9CB0DBAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{613F5BAA-2266-482A-981E-1BA0BCCD14EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3615" yWindow="720" windowWidth="22440" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="600" windowWidth="22440" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Uitleg" sheetId="5" r:id="rId1"/>
@@ -2391,10 +2391,7 @@
       <c r="I32" s="64"/>
       <c r="J32" s="65"/>
       <c r="K32" s="65"/>
-      <c r="L32" s="66" t="str">
-        <f t="shared" ref="L32" si="3">IF(J32&lt;&gt;"",J32+K32,"")</f>
-        <v/>
-      </c>
+      <c r="L32" s="66"/>
       <c r="M32" s="65"/>
       <c r="N32" s="65"/>
       <c r="O32" s="65"/>

</xml_diff>

<commit_message>
Import and publish BK 25m1p individual results
</commit_message>
<xml_diff>
--- a/CompLaagBond/files/template-excel-bk-25m1pijl-indiv.xlsx
+++ b/CompLaagBond/files/template-excel-bk-25m1pijl-indiv.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects Ramon\Websites\NHB-applicaties\Excel programma's\BK excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{613F5BAA-2266-482A-981E-1BA0BCCD14EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8259A4FB-C8F9-46EC-883B-655C6F0F3A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="600" windowWidth="22440" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9465" yWindow="735" windowWidth="16995" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Uitleg" sheetId="5" r:id="rId1"/>
     <sheet name="Wedstrijd" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Wedstrijd!$A$7:$U$31</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Wedstrijd!$C$3:$R$32</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
   <si>
     <t>Bondsnr</t>
   </si>
@@ -33,9 +34,6 @@
   </si>
   <si>
     <t>Vereniging</t>
-  </si>
-  <si>
-    <t>Regio</t>
   </si>
   <si>
     <t>Regio gem.</t>
@@ -290,6 +288,21 @@
   </si>
   <si>
     <t>In kolom R wordt automatisch de uitslag genoteerd: "Bondskampioen", "2e plaats" en "3e plaats".</t>
+  </si>
+  <si>
+    <t>Ver nr</t>
+  </si>
+  <si>
+    <t>Hier komt ver naam</t>
+  </si>
+  <si>
+    <t>Hier komt naam</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Gemiddelde</t>
   </si>
 </sst>
 </file>
@@ -460,7 +473,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -593,10 +606,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -734,6 +743,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1114,7 +1131,7 @@
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="27"/>
     </row>
@@ -1124,20 +1141,20 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" s="30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="27"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="27"/>
       <c r="B5" s="31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="27"/>
       <c r="B6" s="31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1146,14 +1163,14 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="31"/>
     </row>
     <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.2">
       <c r="A9" s="27"/>
       <c r="B9" s="31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1162,20 +1179,20 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="31"/>
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A12" s="27"/>
       <c r="B12" s="31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A13" s="27"/>
       <c r="B13" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1184,14 +1201,14 @@
     </row>
     <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A15" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="27"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="27"/>
       <c r="B16" s="31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1200,20 +1217,20 @@
     </row>
     <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A18" s="30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" s="27"/>
     </row>
     <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A19" s="27"/>
       <c r="B19" s="31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="27"/>
       <c r="B20" s="31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -1222,26 +1239,26 @@
     </row>
     <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A22" s="30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" s="27"/>
     </row>
     <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A23" s="27"/>
       <c r="B23" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="27"/>
       <c r="B24" s="31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" s="27"/>
       <c r="B25" s="31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -1250,20 +1267,20 @@
     </row>
     <row r="27" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A27" s="30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="27"/>
     </row>
     <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A28" s="27"/>
       <c r="B28" s="31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="27"/>
       <c r="B29" s="31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -1272,32 +1289,32 @@
     </row>
     <row r="31" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31" s="32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B31" s="31"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="27"/>
       <c r="B32" s="31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="27"/>
       <c r="B33" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A34" s="30"/>
       <c r="B34" s="27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" s="27"/>
       <c r="B35" s="31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -1306,20 +1323,20 @@
     </row>
     <row r="37" spans="1:2" s="34" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A37" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B37" s="32"/>
     </row>
     <row r="38" spans="1:2" s="34" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A38" s="32"/>
       <c r="B38" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="27"/>
       <c r="B39" s="35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -1351,8 +1368,8 @@
     <col min="3" max="3" width="2.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.85546875" style="14" customWidth="1"/>
     <col min="5" max="5" width="28.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="26.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" style="11" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" style="11" customWidth="1"/>
     <col min="8" max="8" width="26.85546875" style="1" customWidth="1"/>
     <col min="9" max="9" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="5" style="24" customWidth="1"/>
@@ -1370,12 +1387,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="56"/>
+      <c r="A3" s="55"/>
       <c r="B3" s="39"/>
       <c r="C3" s="39"/>
       <c r="D3" s="39"/>
       <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
+      <c r="F3" s="71"/>
       <c r="G3" s="39"/>
       <c r="H3" s="40"/>
       <c r="I3" s="39"/>
@@ -1395,94 +1412,94 @@
     <row r="4" spans="1:25" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="40"/>
       <c r="B4" s="40"/>
-      <c r="C4" s="79" t="str">
+      <c r="C4" s="78" t="str">
         <f>"Bondskampioenschappen 25m1pijl &lt;seizoen&gt;, &lt;klasse&gt;"</f>
         <v>Bondskampioenschappen 25m1pijl &lt;seizoen&gt;, &lt;klasse&gt;</v>
       </c>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="80"/>
-      <c r="J4" s="80"/>
-      <c r="K4" s="80"/>
-      <c r="L4" s="80"/>
-      <c r="M4" s="80"/>
-      <c r="N4" s="80"/>
-      <c r="O4" s="80"/>
-      <c r="P4" s="80"/>
-      <c r="Q4" s="80"/>
-      <c r="R4" s="81"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
+      <c r="L4" s="79"/>
+      <c r="M4" s="79"/>
+      <c r="N4" s="79"/>
+      <c r="O4" s="79"/>
+      <c r="P4" s="79"/>
+      <c r="Q4" s="79"/>
+      <c r="R4" s="80"/>
       <c r="S4" s="40"/>
-      <c r="T4" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="U4" s="57"/>
+      <c r="T4" s="56" t="s">
+        <v>43</v>
+      </c>
+      <c r="U4" s="56"/>
     </row>
     <row r="5" spans="1:25" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="40"/>
       <c r="B5" s="40"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="77" t="s">
+      <c r="C5" s="47"/>
+      <c r="D5" s="76" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="76"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="77"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="44" t="s">
+      <c r="H5" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="84" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="84"/>
-      <c r="J5" s="55"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="77" t="s">
-        <v>54</v>
-      </c>
-      <c r="N5" s="77"/>
-      <c r="O5" s="77"/>
-      <c r="P5" s="77"/>
-      <c r="Q5" s="77"/>
-      <c r="R5" s="78"/>
-      <c r="S5" s="86" t="s">
-        <v>43</v>
-      </c>
-      <c r="T5" s="87"/>
-      <c r="U5" s="87"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="76" t="s">
+        <v>53</v>
+      </c>
+      <c r="N5" s="76"/>
+      <c r="O5" s="76"/>
+      <c r="P5" s="76"/>
+      <c r="Q5" s="76"/>
+      <c r="R5" s="77"/>
+      <c r="S5" s="85" t="s">
+        <v>42</v>
+      </c>
+      <c r="T5" s="86"/>
+      <c r="U5" s="86"/>
     </row>
     <row r="6" spans="1:25" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="40"/>
       <c r="B6" s="40"/>
-      <c r="C6" s="48"/>
+      <c r="C6" s="47"/>
       <c r="D6" s="42"/>
       <c r="E6" s="42"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="85" t="s">
-        <v>36</v>
-      </c>
-      <c r="K6" s="85"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="82" t="s">
-        <v>46</v>
-      </c>
-      <c r="N6" s="82"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="84" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="84"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="81" t="s">
+        <v>45</v>
+      </c>
+      <c r="N6" s="81"/>
       <c r="O6" s="22"/>
-      <c r="P6" s="46"/>
-      <c r="Q6" s="46"/>
-      <c r="R6" s="52"/>
+      <c r="P6" s="45"/>
+      <c r="Q6" s="45"/>
+      <c r="R6" s="51"/>
       <c r="S6" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="T6" s="58"/>
-      <c r="U6" s="58"/>
-      <c r="X6" s="54" t="s">
-        <v>45</v>
+        <v>33</v>
+      </c>
+      <c r="T6" s="57"/>
+      <c r="U6" s="57"/>
+      <c r="X6" s="53" t="s">
+        <v>44</v>
       </c>
       <c r="Y6" s="1" t="b">
         <f>AND(COUNTA(K8:K31)&gt;0,COUNTA(J8:J31)=COUNTA(K8:K31))</f>
@@ -1490,11 +1507,11 @@
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A7" s="83" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="83"/>
-      <c r="C7" s="49">
+      <c r="A7" s="82" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="82"/>
+      <c r="C7" s="48">
         <v>0</v>
       </c>
       <c r="D7" s="6" t="s">
@@ -1503,24 +1520,24 @@
       <c r="E7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>3</v>
-      </c>
       <c r="H7" s="7"/>
-      <c r="I7" s="9" t="s">
-        <v>4</v>
+      <c r="I7" s="88" t="s">
+        <v>61</v>
       </c>
       <c r="J7" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="22" t="s">
-        <v>12</v>
-      </c>
       <c r="L7" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M7" s="22">
         <v>10</v>
@@ -1533,20 +1550,20 @@
       </c>
       <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
-      <c r="R7" s="53" t="s">
+      <c r="R7" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="S7" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="T7" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="U7" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="X7" s="53" t="s">
         <v>37</v>
-      </c>
-      <c r="S7" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="T7" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="U7" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="X7" s="54" t="s">
-        <v>38</v>
       </c>
       <c r="Y7" s="1">
         <f>IF(Y6,IF(LARGE($S$8:$S$31,1)&gt;0,LARGE($S$8:$S$31,1),-1),-2)</f>
@@ -1554,11 +1571,25 @@
       </c>
     </row>
     <row r="8" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="50"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="19"/>
+      <c r="A8" s="53">
+        <v>1</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="49"/>
+      <c r="D8" s="17">
+        <v>100001</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="17">
+        <v>1000</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="H8" s="13"/>
       <c r="I8" s="20"/>
       <c r="J8" s="23"/>
@@ -1572,7 +1603,7 @@
       <c r="O8" s="23"/>
       <c r="P8" s="13"/>
       <c r="Q8" s="13"/>
-      <c r="R8" s="51" t="str">
+      <c r="R8" s="50" t="str">
         <f>IF(S8=$Y$7,"Bondskampioen",IF(S8=$Y$8,"2e plaats",IF(S8=$Y$9,"3e plaats","")))</f>
         <v/>
       </c>
@@ -1584,8 +1615,8 @@
       <c r="U8" s="2"/>
       <c r="V8" s="13"/>
       <c r="W8" s="13"/>
-      <c r="X8" s="54" t="s">
-        <v>39</v>
+      <c r="X8" s="53" t="s">
+        <v>38</v>
       </c>
       <c r="Y8" s="1">
         <f>IF(Y6,IF(LARGE($S$8:$S$31,2)&gt;0,LARGE($S$8:$S$31,2),-1),-2)</f>
@@ -1593,10 +1624,10 @@
       </c>
     </row>
     <row r="9" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="50"/>
+      <c r="C9" s="49"/>
       <c r="D9" s="17"/>
       <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
+      <c r="F9" s="19"/>
       <c r="G9" s="19"/>
       <c r="H9" s="13"/>
       <c r="I9" s="20"/>
@@ -1611,7 +1642,7 @@
       <c r="O9" s="23"/>
       <c r="P9" s="13"/>
       <c r="Q9" s="13"/>
-      <c r="R9" s="51" t="str">
+      <c r="R9" s="50" t="str">
         <f t="shared" ref="R9:R31" si="2">IF(S9=$Y$7,"Bondskampioen",IF(S9=$Y$8,"2e plaats",IF(S9=$Y$9,"3e plaats","")))</f>
         <v/>
       </c>
@@ -1623,8 +1654,8 @@
       <c r="U9" s="12"/>
       <c r="V9" s="13"/>
       <c r="W9" s="13"/>
-      <c r="X9" s="54" t="s">
-        <v>40</v>
+      <c r="X9" s="53" t="s">
+        <v>39</v>
       </c>
       <c r="Y9" s="1">
         <f>IF(Y6,IF(LARGE($S$8:$S$31,3)&gt;0,LARGE($S$8:$S$31,3),-1),-2)</f>
@@ -1634,10 +1665,10 @@
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="18"/>
       <c r="B10" s="18"/>
-      <c r="C10" s="50"/>
+      <c r="C10" s="49"/>
       <c r="D10" s="17"/>
       <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
+      <c r="F10" s="19"/>
       <c r="G10" s="19"/>
       <c r="H10" s="13"/>
       <c r="I10" s="20"/>
@@ -1652,7 +1683,7 @@
       <c r="O10" s="23"/>
       <c r="P10" s="13"/>
       <c r="Q10" s="13"/>
-      <c r="R10" s="51" t="str">
+      <c r="R10" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -1668,10 +1699,10 @@
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
-      <c r="C11" s="50"/>
+      <c r="C11" s="49"/>
       <c r="D11" s="17"/>
       <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
+      <c r="F11" s="19"/>
       <c r="G11" s="19"/>
       <c r="H11" s="13"/>
       <c r="I11" s="20"/>
@@ -1686,7 +1717,7 @@
       <c r="O11" s="23"/>
       <c r="P11" s="13"/>
       <c r="Q11" s="13"/>
-      <c r="R11" s="51" t="str">
+      <c r="R11" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -1702,10 +1733,10 @@
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="18"/>
       <c r="B12" s="18"/>
-      <c r="C12" s="50"/>
+      <c r="C12" s="49"/>
       <c r="D12" s="17"/>
       <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
+      <c r="F12" s="19"/>
       <c r="G12" s="19"/>
       <c r="H12" s="13"/>
       <c r="I12" s="20"/>
@@ -1720,7 +1751,7 @@
       <c r="O12" s="23"/>
       <c r="P12" s="13"/>
       <c r="Q12" s="13"/>
-      <c r="R12" s="51" t="str">
+      <c r="R12" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -1736,10 +1767,10 @@
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
-      <c r="C13" s="50"/>
+      <c r="C13" s="49"/>
       <c r="D13" s="17"/>
       <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
+      <c r="F13" s="19"/>
       <c r="G13" s="19"/>
       <c r="H13" s="13"/>
       <c r="I13" s="20"/>
@@ -1754,7 +1785,7 @@
       <c r="O13" s="23"/>
       <c r="P13" s="13"/>
       <c r="Q13" s="13"/>
-      <c r="R13" s="51" t="str">
+      <c r="R13" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -1770,10 +1801,10 @@
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="18"/>
       <c r="B14" s="18"/>
-      <c r="C14" s="50"/>
+      <c r="C14" s="49"/>
       <c r="D14" s="17"/>
       <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
+      <c r="F14" s="19"/>
       <c r="G14" s="19"/>
       <c r="H14" s="13"/>
       <c r="I14" s="20"/>
@@ -1788,7 +1819,7 @@
       <c r="O14" s="23"/>
       <c r="P14" s="13"/>
       <c r="Q14" s="13"/>
-      <c r="R14" s="51" t="str">
+      <c r="R14" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -1804,10 +1835,10 @@
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="18"/>
       <c r="B15" s="18"/>
-      <c r="C15" s="50"/>
+      <c r="C15" s="49"/>
       <c r="D15" s="17"/>
       <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
+      <c r="F15" s="19"/>
       <c r="G15" s="19"/>
       <c r="H15" s="13"/>
       <c r="I15" s="20"/>
@@ -1822,7 +1853,7 @@
       <c r="O15" s="23"/>
       <c r="P15" s="13"/>
       <c r="Q15" s="13"/>
-      <c r="R15" s="51" t="str">
+      <c r="R15" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -1838,10 +1869,10 @@
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="18"/>
       <c r="B16" s="18"/>
-      <c r="C16" s="50"/>
+      <c r="C16" s="49"/>
       <c r="D16" s="17"/>
       <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
+      <c r="F16" s="19"/>
       <c r="G16" s="19"/>
       <c r="H16" s="13"/>
       <c r="I16" s="20"/>
@@ -1856,7 +1887,7 @@
       <c r="O16" s="23"/>
       <c r="P16" s="13"/>
       <c r="Q16" s="13"/>
-      <c r="R16" s="51" t="str">
+      <c r="R16" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -1872,10 +1903,10 @@
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" s="18"/>
       <c r="B17" s="18"/>
-      <c r="C17" s="50"/>
+      <c r="C17" s="49"/>
       <c r="D17" s="17"/>
       <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
+      <c r="F17" s="19"/>
       <c r="G17" s="19"/>
       <c r="H17" s="13"/>
       <c r="I17" s="20"/>
@@ -1890,7 +1921,7 @@
       <c r="O17" s="23"/>
       <c r="P17" s="13"/>
       <c r="Q17" s="13"/>
-      <c r="R17" s="51" t="str">
+      <c r="R17" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -1906,10 +1937,10 @@
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" s="18"/>
       <c r="B18" s="18"/>
-      <c r="C18" s="50"/>
+      <c r="C18" s="49"/>
       <c r="D18" s="17"/>
       <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
+      <c r="F18" s="19"/>
       <c r="G18" s="19"/>
       <c r="H18" s="13"/>
       <c r="I18" s="20"/>
@@ -1924,7 +1955,7 @@
       <c r="O18" s="23"/>
       <c r="P18" s="13"/>
       <c r="Q18" s="13"/>
-      <c r="R18" s="51" t="str">
+      <c r="R18" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -1940,10 +1971,10 @@
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" s="18"/>
       <c r="B19" s="18"/>
-      <c r="C19" s="50"/>
+      <c r="C19" s="49"/>
       <c r="D19" s="17"/>
       <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
+      <c r="F19" s="19"/>
       <c r="G19" s="19"/>
       <c r="H19" s="13"/>
       <c r="I19" s="20"/>
@@ -1958,7 +1989,7 @@
       <c r="O19" s="23"/>
       <c r="P19" s="13"/>
       <c r="Q19" s="13"/>
-      <c r="R19" s="51" t="str">
+      <c r="R19" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -1974,10 +2005,10 @@
     <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" s="18"/>
       <c r="B20" s="18"/>
-      <c r="C20" s="50"/>
+      <c r="C20" s="49"/>
       <c r="D20" s="17"/>
       <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
+      <c r="F20" s="19"/>
       <c r="G20" s="19"/>
       <c r="H20" s="13"/>
       <c r="I20" s="20"/>
@@ -1992,7 +2023,7 @@
       <c r="O20" s="23"/>
       <c r="P20" s="13"/>
       <c r="Q20" s="13"/>
-      <c r="R20" s="51" t="str">
+      <c r="R20" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2008,10 +2039,10 @@
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" s="18"/>
       <c r="B21" s="18"/>
-      <c r="C21" s="50"/>
+      <c r="C21" s="49"/>
       <c r="D21" s="17"/>
       <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
+      <c r="F21" s="19"/>
       <c r="G21" s="19"/>
       <c r="H21" s="13"/>
       <c r="I21" s="20"/>
@@ -2026,7 +2057,7 @@
       <c r="O21" s="23"/>
       <c r="P21" s="13"/>
       <c r="Q21" s="13"/>
-      <c r="R21" s="51" t="str">
+      <c r="R21" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2042,10 +2073,10 @@
     <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" s="18"/>
       <c r="B22" s="18"/>
-      <c r="C22" s="50"/>
+      <c r="C22" s="49"/>
       <c r="D22" s="17"/>
       <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
+      <c r="F22" s="19"/>
       <c r="G22" s="19"/>
       <c r="H22" s="13"/>
       <c r="I22" s="20"/>
@@ -2060,7 +2091,7 @@
       <c r="O22" s="23"/>
       <c r="P22" s="13"/>
       <c r="Q22" s="13"/>
-      <c r="R22" s="51" t="str">
+      <c r="R22" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2076,10 +2107,10 @@
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
-      <c r="C23" s="50"/>
+      <c r="C23" s="49"/>
       <c r="D23" s="17"/>
       <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
+      <c r="F23" s="19"/>
       <c r="G23" s="19"/>
       <c r="H23" s="13"/>
       <c r="I23" s="20"/>
@@ -2094,7 +2125,7 @@
       <c r="O23" s="23"/>
       <c r="P23" s="13"/>
       <c r="Q23" s="13"/>
-      <c r="R23" s="51" t="str">
+      <c r="R23" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2110,10 +2141,10 @@
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" s="18"/>
       <c r="B24" s="3"/>
-      <c r="C24" s="50"/>
+      <c r="C24" s="49"/>
       <c r="D24" s="15"/>
       <c r="E24"/>
-      <c r="F24"/>
+      <c r="F24" s="16"/>
       <c r="G24" s="16"/>
       <c r="H24"/>
       <c r="I24" s="10"/>
@@ -2128,7 +2159,7 @@
       <c r="O24" s="21"/>
       <c r="P24"/>
       <c r="Q24"/>
-      <c r="R24" s="51" t="str">
+      <c r="R24" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2144,10 +2175,10 @@
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" s="18"/>
       <c r="B25" s="3"/>
-      <c r="C25" s="50"/>
+      <c r="C25" s="49"/>
       <c r="D25" s="15"/>
       <c r="E25"/>
-      <c r="F25"/>
+      <c r="F25" s="16"/>
       <c r="G25" s="16"/>
       <c r="H25"/>
       <c r="I25" s="10"/>
@@ -2162,7 +2193,7 @@
       <c r="O25" s="21"/>
       <c r="P25"/>
       <c r="Q25"/>
-      <c r="R25" s="51" t="str">
+      <c r="R25" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2178,10 +2209,10 @@
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" s="18"/>
       <c r="B26" s="3"/>
-      <c r="C26" s="50"/>
+      <c r="C26" s="49"/>
       <c r="D26" s="15"/>
       <c r="E26"/>
-      <c r="F26"/>
+      <c r="F26" s="16"/>
       <c r="G26" s="16"/>
       <c r="H26"/>
       <c r="I26" s="10"/>
@@ -2196,7 +2227,7 @@
       <c r="O26" s="21"/>
       <c r="P26"/>
       <c r="Q26"/>
-      <c r="R26" s="51" t="str">
+      <c r="R26" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2212,10 +2243,10 @@
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" s="18"/>
       <c r="B27" s="3"/>
-      <c r="C27" s="50"/>
+      <c r="C27" s="49"/>
       <c r="D27" s="15"/>
       <c r="E27"/>
-      <c r="F27"/>
+      <c r="F27" s="16"/>
       <c r="G27" s="16"/>
       <c r="H27"/>
       <c r="I27" s="10"/>
@@ -2230,7 +2261,7 @@
       <c r="O27" s="21"/>
       <c r="P27"/>
       <c r="Q27"/>
-      <c r="R27" s="51" t="str">
+      <c r="R27" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2246,10 +2277,10 @@
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28" s="18"/>
       <c r="B28" s="3"/>
-      <c r="C28" s="50"/>
+      <c r="C28" s="49"/>
       <c r="D28" s="15"/>
       <c r="E28"/>
-      <c r="F28"/>
+      <c r="F28" s="16"/>
       <c r="G28" s="16"/>
       <c r="H28"/>
       <c r="I28" s="10"/>
@@ -2264,7 +2295,7 @@
       <c r="O28" s="21"/>
       <c r="P28"/>
       <c r="Q28"/>
-      <c r="R28" s="51" t="str">
+      <c r="R28" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2280,10 +2311,10 @@
     <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29" s="18"/>
       <c r="B29" s="3"/>
-      <c r="C29" s="50"/>
+      <c r="C29" s="49"/>
       <c r="D29" s="15"/>
       <c r="E29"/>
-      <c r="F29"/>
+      <c r="F29" s="16"/>
       <c r="G29" s="16"/>
       <c r="H29"/>
       <c r="I29" s="10"/>
@@ -2298,7 +2329,7 @@
       <c r="O29" s="21"/>
       <c r="P29"/>
       <c r="Q29"/>
-      <c r="R29" s="51" t="str">
+      <c r="R29" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2314,10 +2345,10 @@
     <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30" s="18"/>
       <c r="B30" s="3"/>
-      <c r="C30" s="50"/>
+      <c r="C30" s="49"/>
       <c r="D30" s="15"/>
       <c r="E30"/>
-      <c r="F30"/>
+      <c r="F30" s="16"/>
       <c r="G30" s="16"/>
       <c r="H30"/>
       <c r="I30" s="10"/>
@@ -2332,7 +2363,7 @@
       <c r="O30" s="21"/>
       <c r="P30"/>
       <c r="Q30"/>
-      <c r="R30" s="51" t="str">
+      <c r="R30" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2348,10 +2379,10 @@
     <row r="31" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18"/>
       <c r="B31" s="3"/>
-      <c r="C31" s="50"/>
+      <c r="C31" s="49"/>
       <c r="D31" s="15"/>
       <c r="E31"/>
-      <c r="F31"/>
+      <c r="F31" s="16"/>
       <c r="G31" s="16"/>
       <c r="H31"/>
       <c r="I31" s="10"/>
@@ -2366,7 +2397,7 @@
       <c r="O31" s="21"/>
       <c r="P31"/>
       <c r="Q31"/>
-      <c r="R31" s="51" t="str">
+      <c r="R31" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2380,24 +2411,24 @@
       <c r="W31"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A32" s="59"/>
-      <c r="B32" s="59"/>
-      <c r="C32" s="60"/>
-      <c r="D32" s="61"/>
-      <c r="E32" s="62"/>
+      <c r="A32" s="58"/>
+      <c r="B32" s="58"/>
+      <c r="C32" s="59"/>
+      <c r="D32" s="60"/>
+      <c r="E32" s="61"/>
       <c r="F32" s="62"/>
-      <c r="G32" s="63"/>
-      <c r="H32" s="62"/>
-      <c r="I32" s="64"/>
-      <c r="J32" s="65"/>
-      <c r="K32" s="65"/>
-      <c r="L32" s="66"/>
-      <c r="M32" s="65"/>
-      <c r="N32" s="65"/>
-      <c r="O32" s="65"/>
-      <c r="P32" s="62"/>
-      <c r="Q32" s="62"/>
-      <c r="R32" s="62"/>
+      <c r="G32" s="62"/>
+      <c r="H32" s="61"/>
+      <c r="I32" s="63"/>
+      <c r="J32" s="64"/>
+      <c r="K32" s="64"/>
+      <c r="L32" s="65"/>
+      <c r="M32" s="64"/>
+      <c r="N32" s="64"/>
+      <c r="O32" s="64"/>
+      <c r="P32" s="61"/>
+      <c r="Q32" s="61"/>
+      <c r="R32" s="61"/>
       <c r="S32" s="39"/>
       <c r="T32" s="38"/>
       <c r="U32" s="38"/>
@@ -2405,34 +2436,34 @@
       <c r="W32"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A33" s="57" t="s">
-        <v>13</v>
+      <c r="A33" s="56" t="s">
+        <v>12</v>
       </c>
       <c r="B33" s="40"/>
       <c r="C33" s="39"/>
-      <c r="D33" s="67"/>
+      <c r="D33" s="66"/>
       <c r="E33" s="39"/>
-      <c r="F33" s="39"/>
-      <c r="G33" s="68" t="s">
-        <v>44</v>
+      <c r="F33" s="71"/>
+      <c r="G33" s="67" t="s">
+        <v>43</v>
       </c>
       <c r="H33" s="39"/>
-      <c r="I33" s="69"/>
+      <c r="I33" s="68"/>
       <c r="J33" s="41"/>
       <c r="K33" s="41"/>
-      <c r="L33" s="70" t="s">
-        <v>41</v>
+      <c r="L33" s="69" t="s">
+        <v>40</v>
       </c>
       <c r="M33" s="41"/>
       <c r="N33" s="41"/>
       <c r="O33" s="41"/>
       <c r="P33" s="39"/>
       <c r="Q33" s="39"/>
-      <c r="R33" s="71" t="s">
-        <v>41</v>
-      </c>
-      <c r="S33" s="71" t="s">
-        <v>41</v>
+      <c r="R33" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="S33" s="70" t="s">
+        <v>40</v>
       </c>
       <c r="T33" s="38"/>
       <c r="U33" s="38"/>
@@ -2440,30 +2471,30 @@
       <c r="W33"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A34" s="59"/>
-      <c r="B34" s="59"/>
+      <c r="A34" s="58"/>
+      <c r="B34" s="58"/>
       <c r="C34" s="39"/>
-      <c r="D34" s="67"/>
+      <c r="D34" s="66"/>
       <c r="E34" s="39"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="72"/>
+      <c r="F34" s="71"/>
+      <c r="G34" s="71"/>
       <c r="H34" s="39"/>
-      <c r="I34" s="69"/>
+      <c r="I34" s="68"/>
       <c r="J34" s="41"/>
       <c r="K34" s="41"/>
-      <c r="L34" s="70" t="s">
-        <v>41</v>
-      </c>
-      <c r="M34" s="73"/>
-      <c r="N34" s="73"/>
-      <c r="O34" s="73"/>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="74"/>
-      <c r="R34" s="71" t="s">
-        <v>41</v>
-      </c>
-      <c r="S34" s="71" t="s">
-        <v>41</v>
+      <c r="L34" s="69" t="s">
+        <v>40</v>
+      </c>
+      <c r="M34" s="72"/>
+      <c r="N34" s="72"/>
+      <c r="O34" s="72"/>
+      <c r="P34" s="73"/>
+      <c r="Q34" s="73"/>
+      <c r="R34" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="S34" s="70" t="s">
+        <v>40</v>
       </c>
       <c r="T34" s="38"/>
       <c r="U34" s="38"/>
@@ -2471,29 +2502,29 @@
       <c r="W34"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A35" s="57" t="s">
-        <v>14</v>
+      <c r="A35" s="56" t="s">
+        <v>13</v>
       </c>
       <c r="B35" s="40"/>
       <c r="C35" s="39"/>
-      <c r="D35" s="75"/>
+      <c r="D35" s="74"/>
       <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
-      <c r="G35" s="72"/>
+      <c r="F35" s="71"/>
+      <c r="G35" s="71"/>
       <c r="H35" s="39"/>
-      <c r="I35" s="69"/>
+      <c r="I35" s="68"/>
       <c r="J35" s="41"/>
       <c r="K35" s="41"/>
-      <c r="L35" s="76" t="s">
-        <v>42</v>
-      </c>
-      <c r="M35" s="76"/>
-      <c r="N35" s="76"/>
-      <c r="O35" s="76"/>
-      <c r="P35" s="76"/>
-      <c r="Q35" s="76"/>
-      <c r="R35" s="76"/>
-      <c r="S35" s="76"/>
+      <c r="L35" s="75" t="s">
+        <v>41</v>
+      </c>
+      <c r="M35" s="75"/>
+      <c r="N35" s="75"/>
+      <c r="O35" s="75"/>
+      <c r="P35" s="75"/>
+      <c r="Q35" s="75"/>
+      <c r="R35" s="75"/>
+      <c r="S35" s="75"/>
       <c r="T35" s="38"/>
       <c r="U35" s="38"/>
       <c r="V35"/>
@@ -2506,21 +2537,21 @@
       <c r="E36" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F36" s="7" t="s">
+      <c r="F36" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G36" s="6" t="s">
         <v>2</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>3</v>
       </c>
       <c r="H36" s="7"/>
       <c r="I36" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T36" s="25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U36" s="25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Small fixes + public BK 25m1p indiv
</commit_message>
<xml_diff>
--- a/CompLaagBond/files/template-excel-bk-25m1pijl-indiv.xlsx
+++ b/CompLaagBond/files/template-excel-bk-25m1pijl-indiv.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects Ramon\Websites\NHB-applicaties\Excel programma's\BK excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{613F5BAA-2266-482A-981E-1BA0BCCD14EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8259A4FB-C8F9-46EC-883B-655C6F0F3A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="600" windowWidth="22440" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9465" yWindow="735" windowWidth="16995" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Uitleg" sheetId="5" r:id="rId1"/>
     <sheet name="Wedstrijd" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Wedstrijd!$A$7:$U$31</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Wedstrijd!$C$3:$R$32</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
   <si>
     <t>Bondsnr</t>
   </si>
@@ -33,9 +34,6 @@
   </si>
   <si>
     <t>Vereniging</t>
-  </si>
-  <si>
-    <t>Regio</t>
   </si>
   <si>
     <t>Regio gem.</t>
@@ -290,6 +288,21 @@
   </si>
   <si>
     <t>In kolom R wordt automatisch de uitslag genoteerd: "Bondskampioen", "2e plaats" en "3e plaats".</t>
+  </si>
+  <si>
+    <t>Ver nr</t>
+  </si>
+  <si>
+    <t>Hier komt ver naam</t>
+  </si>
+  <si>
+    <t>Hier komt naam</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Gemiddelde</t>
   </si>
 </sst>
 </file>
@@ -460,7 +473,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -593,10 +606,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -734,6 +743,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1114,7 +1131,7 @@
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="27"/>
     </row>
@@ -1124,20 +1141,20 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" s="30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="27"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="27"/>
       <c r="B5" s="31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="27"/>
       <c r="B6" s="31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1146,14 +1163,14 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="31"/>
     </row>
     <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.2">
       <c r="A9" s="27"/>
       <c r="B9" s="31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1162,20 +1179,20 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="31"/>
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A12" s="27"/>
       <c r="B12" s="31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A13" s="27"/>
       <c r="B13" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1184,14 +1201,14 @@
     </row>
     <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A15" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="27"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="27"/>
       <c r="B16" s="31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1200,20 +1217,20 @@
     </row>
     <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A18" s="30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" s="27"/>
     </row>
     <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A19" s="27"/>
       <c r="B19" s="31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="27"/>
       <c r="B20" s="31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -1222,26 +1239,26 @@
     </row>
     <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A22" s="30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" s="27"/>
     </row>
     <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A23" s="27"/>
       <c r="B23" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="27"/>
       <c r="B24" s="31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" s="27"/>
       <c r="B25" s="31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -1250,20 +1267,20 @@
     </row>
     <row r="27" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A27" s="30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="27"/>
     </row>
     <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A28" s="27"/>
       <c r="B28" s="31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="27"/>
       <c r="B29" s="31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -1272,32 +1289,32 @@
     </row>
     <row r="31" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31" s="32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B31" s="31"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="27"/>
       <c r="B32" s="31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="27"/>
       <c r="B33" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A34" s="30"/>
       <c r="B34" s="27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" s="27"/>
       <c r="B35" s="31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -1306,20 +1323,20 @@
     </row>
     <row r="37" spans="1:2" s="34" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A37" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B37" s="32"/>
     </row>
     <row r="38" spans="1:2" s="34" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A38" s="32"/>
       <c r="B38" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="27"/>
       <c r="B39" s="35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -1351,8 +1368,8 @@
     <col min="3" max="3" width="2.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.85546875" style="14" customWidth="1"/>
     <col min="5" max="5" width="28.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="26.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" style="11" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" style="11" customWidth="1"/>
     <col min="8" max="8" width="26.85546875" style="1" customWidth="1"/>
     <col min="9" max="9" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="5" style="24" customWidth="1"/>
@@ -1370,12 +1387,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="56"/>
+      <c r="A3" s="55"/>
       <c r="B3" s="39"/>
       <c r="C3" s="39"/>
       <c r="D3" s="39"/>
       <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
+      <c r="F3" s="71"/>
       <c r="G3" s="39"/>
       <c r="H3" s="40"/>
       <c r="I3" s="39"/>
@@ -1395,94 +1412,94 @@
     <row r="4" spans="1:25" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="40"/>
       <c r="B4" s="40"/>
-      <c r="C4" s="79" t="str">
+      <c r="C4" s="78" t="str">
         <f>"Bondskampioenschappen 25m1pijl &lt;seizoen&gt;, &lt;klasse&gt;"</f>
         <v>Bondskampioenschappen 25m1pijl &lt;seizoen&gt;, &lt;klasse&gt;</v>
       </c>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="80"/>
-      <c r="J4" s="80"/>
-      <c r="K4" s="80"/>
-      <c r="L4" s="80"/>
-      <c r="M4" s="80"/>
-      <c r="N4" s="80"/>
-      <c r="O4" s="80"/>
-      <c r="P4" s="80"/>
-      <c r="Q4" s="80"/>
-      <c r="R4" s="81"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
+      <c r="L4" s="79"/>
+      <c r="M4" s="79"/>
+      <c r="N4" s="79"/>
+      <c r="O4" s="79"/>
+      <c r="P4" s="79"/>
+      <c r="Q4" s="79"/>
+      <c r="R4" s="80"/>
       <c r="S4" s="40"/>
-      <c r="T4" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="U4" s="57"/>
+      <c r="T4" s="56" t="s">
+        <v>43</v>
+      </c>
+      <c r="U4" s="56"/>
     </row>
     <row r="5" spans="1:25" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="40"/>
       <c r="B5" s="40"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="77" t="s">
+      <c r="C5" s="47"/>
+      <c r="D5" s="76" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="76"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="77"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="44" t="s">
+      <c r="H5" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="84" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="84"/>
-      <c r="J5" s="55"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="77" t="s">
-        <v>54</v>
-      </c>
-      <c r="N5" s="77"/>
-      <c r="O5" s="77"/>
-      <c r="P5" s="77"/>
-      <c r="Q5" s="77"/>
-      <c r="R5" s="78"/>
-      <c r="S5" s="86" t="s">
-        <v>43</v>
-      </c>
-      <c r="T5" s="87"/>
-      <c r="U5" s="87"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="76" t="s">
+        <v>53</v>
+      </c>
+      <c r="N5" s="76"/>
+      <c r="O5" s="76"/>
+      <c r="P5" s="76"/>
+      <c r="Q5" s="76"/>
+      <c r="R5" s="77"/>
+      <c r="S5" s="85" t="s">
+        <v>42</v>
+      </c>
+      <c r="T5" s="86"/>
+      <c r="U5" s="86"/>
     </row>
     <row r="6" spans="1:25" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="40"/>
       <c r="B6" s="40"/>
-      <c r="C6" s="48"/>
+      <c r="C6" s="47"/>
       <c r="D6" s="42"/>
       <c r="E6" s="42"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="85" t="s">
-        <v>36</v>
-      </c>
-      <c r="K6" s="85"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="82" t="s">
-        <v>46</v>
-      </c>
-      <c r="N6" s="82"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="84" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="84"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="81" t="s">
+        <v>45</v>
+      </c>
+      <c r="N6" s="81"/>
       <c r="O6" s="22"/>
-      <c r="P6" s="46"/>
-      <c r="Q6" s="46"/>
-      <c r="R6" s="52"/>
+      <c r="P6" s="45"/>
+      <c r="Q6" s="45"/>
+      <c r="R6" s="51"/>
       <c r="S6" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="T6" s="58"/>
-      <c r="U6" s="58"/>
-      <c r="X6" s="54" t="s">
-        <v>45</v>
+        <v>33</v>
+      </c>
+      <c r="T6" s="57"/>
+      <c r="U6" s="57"/>
+      <c r="X6" s="53" t="s">
+        <v>44</v>
       </c>
       <c r="Y6" s="1" t="b">
         <f>AND(COUNTA(K8:K31)&gt;0,COUNTA(J8:J31)=COUNTA(K8:K31))</f>
@@ -1490,11 +1507,11 @@
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A7" s="83" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="83"/>
-      <c r="C7" s="49">
+      <c r="A7" s="82" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="82"/>
+      <c r="C7" s="48">
         <v>0</v>
       </c>
       <c r="D7" s="6" t="s">
@@ -1503,24 +1520,24 @@
       <c r="E7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>3</v>
-      </c>
       <c r="H7" s="7"/>
-      <c r="I7" s="9" t="s">
-        <v>4</v>
+      <c r="I7" s="88" t="s">
+        <v>61</v>
       </c>
       <c r="J7" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="22" t="s">
-        <v>12</v>
-      </c>
       <c r="L7" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M7" s="22">
         <v>10</v>
@@ -1533,20 +1550,20 @@
       </c>
       <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
-      <c r="R7" s="53" t="s">
+      <c r="R7" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="S7" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="T7" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="U7" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="X7" s="53" t="s">
         <v>37</v>
-      </c>
-      <c r="S7" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="T7" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="U7" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="X7" s="54" t="s">
-        <v>38</v>
       </c>
       <c r="Y7" s="1">
         <f>IF(Y6,IF(LARGE($S$8:$S$31,1)&gt;0,LARGE($S$8:$S$31,1),-1),-2)</f>
@@ -1554,11 +1571,25 @@
       </c>
     </row>
     <row r="8" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="50"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="19"/>
+      <c r="A8" s="53">
+        <v>1</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="49"/>
+      <c r="D8" s="17">
+        <v>100001</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="17">
+        <v>1000</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="H8" s="13"/>
       <c r="I8" s="20"/>
       <c r="J8" s="23"/>
@@ -1572,7 +1603,7 @@
       <c r="O8" s="23"/>
       <c r="P8" s="13"/>
       <c r="Q8" s="13"/>
-      <c r="R8" s="51" t="str">
+      <c r="R8" s="50" t="str">
         <f>IF(S8=$Y$7,"Bondskampioen",IF(S8=$Y$8,"2e plaats",IF(S8=$Y$9,"3e plaats","")))</f>
         <v/>
       </c>
@@ -1584,8 +1615,8 @@
       <c r="U8" s="2"/>
       <c r="V8" s="13"/>
       <c r="W8" s="13"/>
-      <c r="X8" s="54" t="s">
-        <v>39</v>
+      <c r="X8" s="53" t="s">
+        <v>38</v>
       </c>
       <c r="Y8" s="1">
         <f>IF(Y6,IF(LARGE($S$8:$S$31,2)&gt;0,LARGE($S$8:$S$31,2),-1),-2)</f>
@@ -1593,10 +1624,10 @@
       </c>
     </row>
     <row r="9" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="50"/>
+      <c r="C9" s="49"/>
       <c r="D9" s="17"/>
       <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
+      <c r="F9" s="19"/>
       <c r="G9" s="19"/>
       <c r="H9" s="13"/>
       <c r="I9" s="20"/>
@@ -1611,7 +1642,7 @@
       <c r="O9" s="23"/>
       <c r="P9" s="13"/>
       <c r="Q9" s="13"/>
-      <c r="R9" s="51" t="str">
+      <c r="R9" s="50" t="str">
         <f t="shared" ref="R9:R31" si="2">IF(S9=$Y$7,"Bondskampioen",IF(S9=$Y$8,"2e plaats",IF(S9=$Y$9,"3e plaats","")))</f>
         <v/>
       </c>
@@ -1623,8 +1654,8 @@
       <c r="U9" s="12"/>
       <c r="V9" s="13"/>
       <c r="W9" s="13"/>
-      <c r="X9" s="54" t="s">
-        <v>40</v>
+      <c r="X9" s="53" t="s">
+        <v>39</v>
       </c>
       <c r="Y9" s="1">
         <f>IF(Y6,IF(LARGE($S$8:$S$31,3)&gt;0,LARGE($S$8:$S$31,3),-1),-2)</f>
@@ -1634,10 +1665,10 @@
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="18"/>
       <c r="B10" s="18"/>
-      <c r="C10" s="50"/>
+      <c r="C10" s="49"/>
       <c r="D10" s="17"/>
       <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
+      <c r="F10" s="19"/>
       <c r="G10" s="19"/>
       <c r="H10" s="13"/>
       <c r="I10" s="20"/>
@@ -1652,7 +1683,7 @@
       <c r="O10" s="23"/>
       <c r="P10" s="13"/>
       <c r="Q10" s="13"/>
-      <c r="R10" s="51" t="str">
+      <c r="R10" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -1668,10 +1699,10 @@
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
-      <c r="C11" s="50"/>
+      <c r="C11" s="49"/>
       <c r="D11" s="17"/>
       <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
+      <c r="F11" s="19"/>
       <c r="G11" s="19"/>
       <c r="H11" s="13"/>
       <c r="I11" s="20"/>
@@ -1686,7 +1717,7 @@
       <c r="O11" s="23"/>
       <c r="P11" s="13"/>
       <c r="Q11" s="13"/>
-      <c r="R11" s="51" t="str">
+      <c r="R11" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -1702,10 +1733,10 @@
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="18"/>
       <c r="B12" s="18"/>
-      <c r="C12" s="50"/>
+      <c r="C12" s="49"/>
       <c r="D12" s="17"/>
       <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
+      <c r="F12" s="19"/>
       <c r="G12" s="19"/>
       <c r="H12" s="13"/>
       <c r="I12" s="20"/>
@@ -1720,7 +1751,7 @@
       <c r="O12" s="23"/>
       <c r="P12" s="13"/>
       <c r="Q12" s="13"/>
-      <c r="R12" s="51" t="str">
+      <c r="R12" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -1736,10 +1767,10 @@
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
-      <c r="C13" s="50"/>
+      <c r="C13" s="49"/>
       <c r="D13" s="17"/>
       <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
+      <c r="F13" s="19"/>
       <c r="G13" s="19"/>
       <c r="H13" s="13"/>
       <c r="I13" s="20"/>
@@ -1754,7 +1785,7 @@
       <c r="O13" s="23"/>
       <c r="P13" s="13"/>
       <c r="Q13" s="13"/>
-      <c r="R13" s="51" t="str">
+      <c r="R13" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -1770,10 +1801,10 @@
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="18"/>
       <c r="B14" s="18"/>
-      <c r="C14" s="50"/>
+      <c r="C14" s="49"/>
       <c r="D14" s="17"/>
       <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
+      <c r="F14" s="19"/>
       <c r="G14" s="19"/>
       <c r="H14" s="13"/>
       <c r="I14" s="20"/>
@@ -1788,7 +1819,7 @@
       <c r="O14" s="23"/>
       <c r="P14" s="13"/>
       <c r="Q14" s="13"/>
-      <c r="R14" s="51" t="str">
+      <c r="R14" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -1804,10 +1835,10 @@
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="18"/>
       <c r="B15" s="18"/>
-      <c r="C15" s="50"/>
+      <c r="C15" s="49"/>
       <c r="D15" s="17"/>
       <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
+      <c r="F15" s="19"/>
       <c r="G15" s="19"/>
       <c r="H15" s="13"/>
       <c r="I15" s="20"/>
@@ -1822,7 +1853,7 @@
       <c r="O15" s="23"/>
       <c r="P15" s="13"/>
       <c r="Q15" s="13"/>
-      <c r="R15" s="51" t="str">
+      <c r="R15" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -1838,10 +1869,10 @@
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="18"/>
       <c r="B16" s="18"/>
-      <c r="C16" s="50"/>
+      <c r="C16" s="49"/>
       <c r="D16" s="17"/>
       <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
+      <c r="F16" s="19"/>
       <c r="G16" s="19"/>
       <c r="H16" s="13"/>
       <c r="I16" s="20"/>
@@ -1856,7 +1887,7 @@
       <c r="O16" s="23"/>
       <c r="P16" s="13"/>
       <c r="Q16" s="13"/>
-      <c r="R16" s="51" t="str">
+      <c r="R16" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -1872,10 +1903,10 @@
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" s="18"/>
       <c r="B17" s="18"/>
-      <c r="C17" s="50"/>
+      <c r="C17" s="49"/>
       <c r="D17" s="17"/>
       <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
+      <c r="F17" s="19"/>
       <c r="G17" s="19"/>
       <c r="H17" s="13"/>
       <c r="I17" s="20"/>
@@ -1890,7 +1921,7 @@
       <c r="O17" s="23"/>
       <c r="P17" s="13"/>
       <c r="Q17" s="13"/>
-      <c r="R17" s="51" t="str">
+      <c r="R17" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -1906,10 +1937,10 @@
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" s="18"/>
       <c r="B18" s="18"/>
-      <c r="C18" s="50"/>
+      <c r="C18" s="49"/>
       <c r="D18" s="17"/>
       <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
+      <c r="F18" s="19"/>
       <c r="G18" s="19"/>
       <c r="H18" s="13"/>
       <c r="I18" s="20"/>
@@ -1924,7 +1955,7 @@
       <c r="O18" s="23"/>
       <c r="P18" s="13"/>
       <c r="Q18" s="13"/>
-      <c r="R18" s="51" t="str">
+      <c r="R18" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -1940,10 +1971,10 @@
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" s="18"/>
       <c r="B19" s="18"/>
-      <c r="C19" s="50"/>
+      <c r="C19" s="49"/>
       <c r="D19" s="17"/>
       <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
+      <c r="F19" s="19"/>
       <c r="G19" s="19"/>
       <c r="H19" s="13"/>
       <c r="I19" s="20"/>
@@ -1958,7 +1989,7 @@
       <c r="O19" s="23"/>
       <c r="P19" s="13"/>
       <c r="Q19" s="13"/>
-      <c r="R19" s="51" t="str">
+      <c r="R19" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -1974,10 +2005,10 @@
     <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" s="18"/>
       <c r="B20" s="18"/>
-      <c r="C20" s="50"/>
+      <c r="C20" s="49"/>
       <c r="D20" s="17"/>
       <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
+      <c r="F20" s="19"/>
       <c r="G20" s="19"/>
       <c r="H20" s="13"/>
       <c r="I20" s="20"/>
@@ -1992,7 +2023,7 @@
       <c r="O20" s="23"/>
       <c r="P20" s="13"/>
       <c r="Q20" s="13"/>
-      <c r="R20" s="51" t="str">
+      <c r="R20" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2008,10 +2039,10 @@
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" s="18"/>
       <c r="B21" s="18"/>
-      <c r="C21" s="50"/>
+      <c r="C21" s="49"/>
       <c r="D21" s="17"/>
       <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
+      <c r="F21" s="19"/>
       <c r="G21" s="19"/>
       <c r="H21" s="13"/>
       <c r="I21" s="20"/>
@@ -2026,7 +2057,7 @@
       <c r="O21" s="23"/>
       <c r="P21" s="13"/>
       <c r="Q21" s="13"/>
-      <c r="R21" s="51" t="str">
+      <c r="R21" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2042,10 +2073,10 @@
     <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" s="18"/>
       <c r="B22" s="18"/>
-      <c r="C22" s="50"/>
+      <c r="C22" s="49"/>
       <c r="D22" s="17"/>
       <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
+      <c r="F22" s="19"/>
       <c r="G22" s="19"/>
       <c r="H22" s="13"/>
       <c r="I22" s="20"/>
@@ -2060,7 +2091,7 @@
       <c r="O22" s="23"/>
       <c r="P22" s="13"/>
       <c r="Q22" s="13"/>
-      <c r="R22" s="51" t="str">
+      <c r="R22" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2076,10 +2107,10 @@
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
-      <c r="C23" s="50"/>
+      <c r="C23" s="49"/>
       <c r="D23" s="17"/>
       <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
+      <c r="F23" s="19"/>
       <c r="G23" s="19"/>
       <c r="H23" s="13"/>
       <c r="I23" s="20"/>
@@ -2094,7 +2125,7 @@
       <c r="O23" s="23"/>
       <c r="P23" s="13"/>
       <c r="Q23" s="13"/>
-      <c r="R23" s="51" t="str">
+      <c r="R23" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2110,10 +2141,10 @@
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" s="18"/>
       <c r="B24" s="3"/>
-      <c r="C24" s="50"/>
+      <c r="C24" s="49"/>
       <c r="D24" s="15"/>
       <c r="E24"/>
-      <c r="F24"/>
+      <c r="F24" s="16"/>
       <c r="G24" s="16"/>
       <c r="H24"/>
       <c r="I24" s="10"/>
@@ -2128,7 +2159,7 @@
       <c r="O24" s="21"/>
       <c r="P24"/>
       <c r="Q24"/>
-      <c r="R24" s="51" t="str">
+      <c r="R24" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2144,10 +2175,10 @@
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" s="18"/>
       <c r="B25" s="3"/>
-      <c r="C25" s="50"/>
+      <c r="C25" s="49"/>
       <c r="D25" s="15"/>
       <c r="E25"/>
-      <c r="F25"/>
+      <c r="F25" s="16"/>
       <c r="G25" s="16"/>
       <c r="H25"/>
       <c r="I25" s="10"/>
@@ -2162,7 +2193,7 @@
       <c r="O25" s="21"/>
       <c r="P25"/>
       <c r="Q25"/>
-      <c r="R25" s="51" t="str">
+      <c r="R25" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2178,10 +2209,10 @@
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" s="18"/>
       <c r="B26" s="3"/>
-      <c r="C26" s="50"/>
+      <c r="C26" s="49"/>
       <c r="D26" s="15"/>
       <c r="E26"/>
-      <c r="F26"/>
+      <c r="F26" s="16"/>
       <c r="G26" s="16"/>
       <c r="H26"/>
       <c r="I26" s="10"/>
@@ -2196,7 +2227,7 @@
       <c r="O26" s="21"/>
       <c r="P26"/>
       <c r="Q26"/>
-      <c r="R26" s="51" t="str">
+      <c r="R26" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2212,10 +2243,10 @@
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" s="18"/>
       <c r="B27" s="3"/>
-      <c r="C27" s="50"/>
+      <c r="C27" s="49"/>
       <c r="D27" s="15"/>
       <c r="E27"/>
-      <c r="F27"/>
+      <c r="F27" s="16"/>
       <c r="G27" s="16"/>
       <c r="H27"/>
       <c r="I27" s="10"/>
@@ -2230,7 +2261,7 @@
       <c r="O27" s="21"/>
       <c r="P27"/>
       <c r="Q27"/>
-      <c r="R27" s="51" t="str">
+      <c r="R27" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2246,10 +2277,10 @@
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28" s="18"/>
       <c r="B28" s="3"/>
-      <c r="C28" s="50"/>
+      <c r="C28" s="49"/>
       <c r="D28" s="15"/>
       <c r="E28"/>
-      <c r="F28"/>
+      <c r="F28" s="16"/>
       <c r="G28" s="16"/>
       <c r="H28"/>
       <c r="I28" s="10"/>
@@ -2264,7 +2295,7 @@
       <c r="O28" s="21"/>
       <c r="P28"/>
       <c r="Q28"/>
-      <c r="R28" s="51" t="str">
+      <c r="R28" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2280,10 +2311,10 @@
     <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29" s="18"/>
       <c r="B29" s="3"/>
-      <c r="C29" s="50"/>
+      <c r="C29" s="49"/>
       <c r="D29" s="15"/>
       <c r="E29"/>
-      <c r="F29"/>
+      <c r="F29" s="16"/>
       <c r="G29" s="16"/>
       <c r="H29"/>
       <c r="I29" s="10"/>
@@ -2298,7 +2329,7 @@
       <c r="O29" s="21"/>
       <c r="P29"/>
       <c r="Q29"/>
-      <c r="R29" s="51" t="str">
+      <c r="R29" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2314,10 +2345,10 @@
     <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30" s="18"/>
       <c r="B30" s="3"/>
-      <c r="C30" s="50"/>
+      <c r="C30" s="49"/>
       <c r="D30" s="15"/>
       <c r="E30"/>
-      <c r="F30"/>
+      <c r="F30" s="16"/>
       <c r="G30" s="16"/>
       <c r="H30"/>
       <c r="I30" s="10"/>
@@ -2332,7 +2363,7 @@
       <c r="O30" s="21"/>
       <c r="P30"/>
       <c r="Q30"/>
-      <c r="R30" s="51" t="str">
+      <c r="R30" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2348,10 +2379,10 @@
     <row r="31" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18"/>
       <c r="B31" s="3"/>
-      <c r="C31" s="50"/>
+      <c r="C31" s="49"/>
       <c r="D31" s="15"/>
       <c r="E31"/>
-      <c r="F31"/>
+      <c r="F31" s="16"/>
       <c r="G31" s="16"/>
       <c r="H31"/>
       <c r="I31" s="10"/>
@@ -2366,7 +2397,7 @@
       <c r="O31" s="21"/>
       <c r="P31"/>
       <c r="Q31"/>
-      <c r="R31" s="51" t="str">
+      <c r="R31" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2380,24 +2411,24 @@
       <c r="W31"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A32" s="59"/>
-      <c r="B32" s="59"/>
-      <c r="C32" s="60"/>
-      <c r="D32" s="61"/>
-      <c r="E32" s="62"/>
+      <c r="A32" s="58"/>
+      <c r="B32" s="58"/>
+      <c r="C32" s="59"/>
+      <c r="D32" s="60"/>
+      <c r="E32" s="61"/>
       <c r="F32" s="62"/>
-      <c r="G32" s="63"/>
-      <c r="H32" s="62"/>
-      <c r="I32" s="64"/>
-      <c r="J32" s="65"/>
-      <c r="K32" s="65"/>
-      <c r="L32" s="66"/>
-      <c r="M32" s="65"/>
-      <c r="N32" s="65"/>
-      <c r="O32" s="65"/>
-      <c r="P32" s="62"/>
-      <c r="Q32" s="62"/>
-      <c r="R32" s="62"/>
+      <c r="G32" s="62"/>
+      <c r="H32" s="61"/>
+      <c r="I32" s="63"/>
+      <c r="J32" s="64"/>
+      <c r="K32" s="64"/>
+      <c r="L32" s="65"/>
+      <c r="M32" s="64"/>
+      <c r="N32" s="64"/>
+      <c r="O32" s="64"/>
+      <c r="P32" s="61"/>
+      <c r="Q32" s="61"/>
+      <c r="R32" s="61"/>
       <c r="S32" s="39"/>
       <c r="T32" s="38"/>
       <c r="U32" s="38"/>
@@ -2405,34 +2436,34 @@
       <c r="W32"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A33" s="57" t="s">
-        <v>13</v>
+      <c r="A33" s="56" t="s">
+        <v>12</v>
       </c>
       <c r="B33" s="40"/>
       <c r="C33" s="39"/>
-      <c r="D33" s="67"/>
+      <c r="D33" s="66"/>
       <c r="E33" s="39"/>
-      <c r="F33" s="39"/>
-      <c r="G33" s="68" t="s">
-        <v>44</v>
+      <c r="F33" s="71"/>
+      <c r="G33" s="67" t="s">
+        <v>43</v>
       </c>
       <c r="H33" s="39"/>
-      <c r="I33" s="69"/>
+      <c r="I33" s="68"/>
       <c r="J33" s="41"/>
       <c r="K33" s="41"/>
-      <c r="L33" s="70" t="s">
-        <v>41</v>
+      <c r="L33" s="69" t="s">
+        <v>40</v>
       </c>
       <c r="M33" s="41"/>
       <c r="N33" s="41"/>
       <c r="O33" s="41"/>
       <c r="P33" s="39"/>
       <c r="Q33" s="39"/>
-      <c r="R33" s="71" t="s">
-        <v>41</v>
-      </c>
-      <c r="S33" s="71" t="s">
-        <v>41</v>
+      <c r="R33" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="S33" s="70" t="s">
+        <v>40</v>
       </c>
       <c r="T33" s="38"/>
       <c r="U33" s="38"/>
@@ -2440,30 +2471,30 @@
       <c r="W33"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A34" s="59"/>
-      <c r="B34" s="59"/>
+      <c r="A34" s="58"/>
+      <c r="B34" s="58"/>
       <c r="C34" s="39"/>
-      <c r="D34" s="67"/>
+      <c r="D34" s="66"/>
       <c r="E34" s="39"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="72"/>
+      <c r="F34" s="71"/>
+      <c r="G34" s="71"/>
       <c r="H34" s="39"/>
-      <c r="I34" s="69"/>
+      <c r="I34" s="68"/>
       <c r="J34" s="41"/>
       <c r="K34" s="41"/>
-      <c r="L34" s="70" t="s">
-        <v>41</v>
-      </c>
-      <c r="M34" s="73"/>
-      <c r="N34" s="73"/>
-      <c r="O34" s="73"/>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="74"/>
-      <c r="R34" s="71" t="s">
-        <v>41</v>
-      </c>
-      <c r="S34" s="71" t="s">
-        <v>41</v>
+      <c r="L34" s="69" t="s">
+        <v>40</v>
+      </c>
+      <c r="M34" s="72"/>
+      <c r="N34" s="72"/>
+      <c r="O34" s="72"/>
+      <c r="P34" s="73"/>
+      <c r="Q34" s="73"/>
+      <c r="R34" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="S34" s="70" t="s">
+        <v>40</v>
       </c>
       <c r="T34" s="38"/>
       <c r="U34" s="38"/>
@@ -2471,29 +2502,29 @@
       <c r="W34"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A35" s="57" t="s">
-        <v>14</v>
+      <c r="A35" s="56" t="s">
+        <v>13</v>
       </c>
       <c r="B35" s="40"/>
       <c r="C35" s="39"/>
-      <c r="D35" s="75"/>
+      <c r="D35" s="74"/>
       <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
-      <c r="G35" s="72"/>
+      <c r="F35" s="71"/>
+      <c r="G35" s="71"/>
       <c r="H35" s="39"/>
-      <c r="I35" s="69"/>
+      <c r="I35" s="68"/>
       <c r="J35" s="41"/>
       <c r="K35" s="41"/>
-      <c r="L35" s="76" t="s">
-        <v>42</v>
-      </c>
-      <c r="M35" s="76"/>
-      <c r="N35" s="76"/>
-      <c r="O35" s="76"/>
-      <c r="P35" s="76"/>
-      <c r="Q35" s="76"/>
-      <c r="R35" s="76"/>
-      <c r="S35" s="76"/>
+      <c r="L35" s="75" t="s">
+        <v>41</v>
+      </c>
+      <c r="M35" s="75"/>
+      <c r="N35" s="75"/>
+      <c r="O35" s="75"/>
+      <c r="P35" s="75"/>
+      <c r="Q35" s="75"/>
+      <c r="R35" s="75"/>
+      <c r="S35" s="75"/>
       <c r="T35" s="38"/>
       <c r="U35" s="38"/>
       <c r="V35"/>
@@ -2506,21 +2537,21 @@
       <c r="E36" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F36" s="7" t="s">
+      <c r="F36" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G36" s="6" t="s">
         <v>2</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>3</v>
       </c>
       <c r="H36" s="7"/>
       <c r="I36" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T36" s="25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U36" s="25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated all RK/BK programs
</commit_message>
<xml_diff>
--- a/CompLaagBond/files/template-excel-bk-25m1pijl-indiv.xlsx
+++ b/CompLaagBond/files/template-excel-bk-25m1pijl-indiv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects Ramon\Websites\NHB-applicaties\Excel programma's\BK excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8259A4FB-C8F9-46EC-883B-655C6F0F3A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0208B255-DE02-4673-95E0-9093CD4912E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9465" yWindow="735" windowWidth="16995" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5535" yWindow="1350" windowWidth="18195" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Uitleg" sheetId="5" r:id="rId1"/>
@@ -124,9 +124,6 @@
   </si>
   <si>
     <t>Contactgegevens</t>
-  </si>
-  <si>
-    <t>E-mail voor het insturen van de uitslagen: nhb-apps-support@handboogsport.nl</t>
   </si>
   <si>
     <t>E-mail bondsbureau: info@handboogsport.nl</t>
@@ -304,6 +301,28 @@
   <si>
     <t>Gemiddelde</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">E-mail </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>insturen ingevuld bestand</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: mh-support@handboogsport.nl</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -312,7 +331,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -374,6 +393,12 @@
     <font>
       <b/>
       <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -473,7 +498,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -697,6 +722,15 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -743,14 +777,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -794,9 +820,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -834,9 +860,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -869,26 +895,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -921,26 +930,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1131,7 +1123,7 @@
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="27"/>
     </row>
@@ -1179,7 +1171,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="31"/>
     </row>
@@ -1192,7 +1184,7 @@
     <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A13" s="27"/>
       <c r="B13" s="31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1230,7 +1222,7 @@
     <row r="20" spans="1:2" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="27"/>
       <c r="B20" s="31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -1246,19 +1238,19 @@
     <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A23" s="27"/>
       <c r="B23" s="31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="27"/>
       <c r="B24" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" s="27"/>
       <c r="B25" s="31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -1274,13 +1266,13 @@
     <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A28" s="27"/>
       <c r="B28" s="31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="27"/>
       <c r="B29" s="31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -1289,32 +1281,32 @@
     </row>
     <row r="31" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31" s="32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31" s="31"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="27"/>
       <c r="B32" s="31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="27"/>
       <c r="B33" s="31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A34" s="30"/>
       <c r="B34" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" s="27"/>
       <c r="B35" s="31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -1329,14 +1321,14 @@
     </row>
     <row r="38" spans="1:2" s="34" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A38" s="32"/>
-      <c r="B38" s="31" t="s">
-        <v>27</v>
+      <c r="B38" s="77" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="27"/>
       <c r="B39" s="35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -1412,28 +1404,28 @@
     <row r="4" spans="1:25" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="40"/>
       <c r="B4" s="40"/>
-      <c r="C4" s="78" t="str">
+      <c r="C4" s="81" t="str">
         <f>"Bondskampioenschappen 25m1pijl &lt;seizoen&gt;, &lt;klasse&gt;"</f>
         <v>Bondskampioenschappen 25m1pijl &lt;seizoen&gt;, &lt;klasse&gt;</v>
       </c>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="79"/>
-      <c r="J4" s="79"/>
-      <c r="K4" s="79"/>
-      <c r="L4" s="79"/>
-      <c r="M4" s="79"/>
-      <c r="N4" s="79"/>
-      <c r="O4" s="79"/>
-      <c r="P4" s="79"/>
-      <c r="Q4" s="79"/>
-      <c r="R4" s="80"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="82"/>
+      <c r="J4" s="82"/>
+      <c r="K4" s="82"/>
+      <c r="L4" s="82"/>
+      <c r="M4" s="82"/>
+      <c r="N4" s="82"/>
+      <c r="O4" s="82"/>
+      <c r="P4" s="82"/>
+      <c r="Q4" s="82"/>
+      <c r="R4" s="83"/>
       <c r="S4" s="40"/>
       <c r="T4" s="56" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U4" s="56"/>
     </row>
@@ -1441,34 +1433,34 @@
       <c r="A5" s="40"/>
       <c r="B5" s="40"/>
       <c r="C5" s="47"/>
-      <c r="D5" s="76" t="s">
+      <c r="D5" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="76"/>
-      <c r="F5" s="87"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="75"/>
       <c r="G5" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="83" t="s">
+      <c r="H5" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="83"/>
+      <c r="I5" s="86"/>
       <c r="J5" s="54"/>
       <c r="K5" s="46"/>
       <c r="L5" s="46"/>
-      <c r="M5" s="76" t="s">
-        <v>53</v>
-      </c>
-      <c r="N5" s="76"/>
-      <c r="O5" s="76"/>
-      <c r="P5" s="76"/>
-      <c r="Q5" s="76"/>
-      <c r="R5" s="77"/>
-      <c r="S5" s="85" t="s">
-        <v>42</v>
-      </c>
-      <c r="T5" s="86"/>
-      <c r="U5" s="86"/>
+      <c r="M5" s="79" t="s">
+        <v>52</v>
+      </c>
+      <c r="N5" s="79"/>
+      <c r="O5" s="79"/>
+      <c r="P5" s="79"/>
+      <c r="Q5" s="79"/>
+      <c r="R5" s="80"/>
+      <c r="S5" s="88" t="s">
+        <v>41</v>
+      </c>
+      <c r="T5" s="89"/>
+      <c r="U5" s="89"/>
     </row>
     <row r="6" spans="1:25" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="40"/>
@@ -1476,30 +1468,30 @@
       <c r="C6" s="47"/>
       <c r="D6" s="42"/>
       <c r="E6" s="42"/>
-      <c r="F6" s="87"/>
+      <c r="F6" s="75"/>
       <c r="G6" s="43"/>
       <c r="H6" s="44"/>
       <c r="I6" s="44"/>
-      <c r="J6" s="84" t="s">
-        <v>35</v>
-      </c>
-      <c r="K6" s="84"/>
+      <c r="J6" s="87" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" s="87"/>
       <c r="L6" s="46"/>
-      <c r="M6" s="81" t="s">
-        <v>45</v>
-      </c>
-      <c r="N6" s="81"/>
+      <c r="M6" s="84" t="s">
+        <v>44</v>
+      </c>
+      <c r="N6" s="84"/>
       <c r="O6" s="22"/>
       <c r="P6" s="45"/>
       <c r="Q6" s="45"/>
       <c r="R6" s="51"/>
       <c r="S6" s="37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T6" s="57"/>
       <c r="U6" s="57"/>
       <c r="X6" s="53" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Y6" s="1" t="b">
         <f>AND(COUNTA(K8:K31)&gt;0,COUNTA(J8:J31)=COUNTA(K8:K31))</f>
@@ -1507,10 +1499,10 @@
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A7" s="82" t="s">
+      <c r="A7" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="82"/>
+      <c r="B7" s="85"/>
       <c r="C7" s="48">
         <v>0</v>
       </c>
@@ -1521,14 +1513,14 @@
         <v>1</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>2</v>
       </c>
       <c r="H7" s="7"/>
-      <c r="I7" s="88" t="s">
-        <v>61</v>
+      <c r="I7" s="76" t="s">
+        <v>60</v>
       </c>
       <c r="J7" s="22" t="s">
         <v>10</v>
@@ -1537,7 +1529,7 @@
         <v>11</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M7" s="22">
         <v>10</v>
@@ -1551,10 +1543,10 @@
       <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
       <c r="R7" s="52" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S7" s="37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="T7" s="25" t="s">
         <v>5</v>
@@ -1563,7 +1555,7 @@
         <v>14</v>
       </c>
       <c r="X7" s="53" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Y7" s="1">
         <f>IF(Y6,IF(LARGE($S$8:$S$31,1)&gt;0,LARGE($S$8:$S$31,1),-1),-2)</f>
@@ -1575,20 +1567,20 @@
         <v>1</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="49"/>
       <c r="D8" s="17">
         <v>100001</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F8" s="17">
         <v>1000</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H8" s="13"/>
       <c r="I8" s="20"/>
@@ -1616,7 +1608,7 @@
       <c r="V8" s="13"/>
       <c r="W8" s="13"/>
       <c r="X8" s="53" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y8" s="1">
         <f>IF(Y6,IF(LARGE($S$8:$S$31,2)&gt;0,LARGE($S$8:$S$31,2),-1),-2)</f>
@@ -1655,7 +1647,7 @@
       <c r="V9" s="13"/>
       <c r="W9" s="13"/>
       <c r="X9" s="53" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Y9" s="1">
         <f>IF(Y6,IF(LARGE($S$8:$S$31,3)&gt;0,LARGE($S$8:$S$31,3),-1),-2)</f>
@@ -2445,14 +2437,14 @@
       <c r="E33" s="39"/>
       <c r="F33" s="71"/>
       <c r="G33" s="67" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H33" s="39"/>
       <c r="I33" s="68"/>
       <c r="J33" s="41"/>
       <c r="K33" s="41"/>
       <c r="L33" s="69" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M33" s="41"/>
       <c r="N33" s="41"/>
@@ -2460,10 +2452,10 @@
       <c r="P33" s="39"/>
       <c r="Q33" s="39"/>
       <c r="R33" s="70" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="S33" s="70" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T33" s="38"/>
       <c r="U33" s="38"/>
@@ -2483,7 +2475,7 @@
       <c r="J34" s="41"/>
       <c r="K34" s="41"/>
       <c r="L34" s="69" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M34" s="72"/>
       <c r="N34" s="72"/>
@@ -2491,10 +2483,10 @@
       <c r="P34" s="73"/>
       <c r="Q34" s="73"/>
       <c r="R34" s="70" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="S34" s="70" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T34" s="38"/>
       <c r="U34" s="38"/>
@@ -2515,16 +2507,16 @@
       <c r="I35" s="68"/>
       <c r="J35" s="41"/>
       <c r="K35" s="41"/>
-      <c r="L35" s="75" t="s">
-        <v>41</v>
-      </c>
-      <c r="M35" s="75"/>
-      <c r="N35" s="75"/>
-      <c r="O35" s="75"/>
-      <c r="P35" s="75"/>
-      <c r="Q35" s="75"/>
-      <c r="R35" s="75"/>
-      <c r="S35" s="75"/>
+      <c r="L35" s="78" t="s">
+        <v>40</v>
+      </c>
+      <c r="M35" s="78"/>
+      <c r="N35" s="78"/>
+      <c r="O35" s="78"/>
+      <c r="P35" s="78"/>
+      <c r="Q35" s="78"/>
+      <c r="R35" s="78"/>
+      <c r="S35" s="78"/>
       <c r="T35" s="38"/>
       <c r="U35" s="38"/>
       <c r="V35"/>
@@ -2538,7 +2530,7 @@
         <v>1</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Support for 64 archers in BK 25m1pijl
</commit_message>
<xml_diff>
--- a/CompLaagBond/files/template-excel-bk-25m1pijl-indiv.xlsx
+++ b/CompLaagBond/files/template-excel-bk-25m1pijl-indiv.xlsx
@@ -1,31 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects Ramon\Websites\NHB-applicaties\Excel programma's\BK excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0208B255-DE02-4673-95E0-9093CD4912E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC72669-9283-4A94-BE1B-E502A58777EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5535" yWindow="1350" windowWidth="18195" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="23715" windowHeight="14025" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Uitleg" sheetId="5" r:id="rId1"/>
     <sheet name="Wedstrijd" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Wedstrijd!$A$7:$U$31</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Wedstrijd!$C$3:$R$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Wedstrijd!$A$7:$U$71</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Wedstrijd!$C$3:$R$72</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
   <si>
     <t>Bondsnr</t>
   </si>
@@ -182,9 +182,6 @@
   </si>
   <si>
     <t>pas op: formules!</t>
-  </si>
-  <si>
-    <t>Sorteren: selecteer A6 tot en met T29. Menu: sorteer, aflopend op kolom S.</t>
   </si>
   <si>
     <t>Afdrukken: Ctrl+P</t>
@@ -322,6 +319,9 @@
       </rPr>
       <t>: mh-support@handboogsport.nl</t>
     </r>
+  </si>
+  <si>
+    <t>Sorteren: selecteer A8 tot en met T71. Menu: sorteer, aflopend op kolom S.</t>
   </si>
 </sst>
 </file>
@@ -1108,7 +1108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A6380CA-469D-4A31-B933-BC719C1B440A}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1222,7 +1222,7 @@
     <row r="20" spans="1:2" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="27"/>
       <c r="B20" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -1238,19 +1238,19 @@
     <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A23" s="27"/>
       <c r="B23" s="31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="27"/>
       <c r="B24" s="31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" s="27"/>
       <c r="B25" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -1266,13 +1266,13 @@
     <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A28" s="27"/>
       <c r="B28" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="27"/>
       <c r="B29" s="31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -1288,25 +1288,25 @@
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="27"/>
       <c r="B32" s="31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="27"/>
       <c r="B33" s="31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A34" s="30"/>
       <c r="B34" s="27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" s="27"/>
       <c r="B35" s="31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -1322,7 +1322,7 @@
     <row r="38" spans="1:2" s="34" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A38" s="32"/>
       <c r="B38" s="77" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -1347,10 +1347,10 @@
   <sheetPr codeName="Blad1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A3:Y252"/>
+  <dimension ref="A3:Y294"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -1425,7 +1425,7 @@
       <c r="R4" s="83"/>
       <c r="S4" s="40"/>
       <c r="T4" s="56" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="U4" s="56"/>
     </row>
@@ -1449,7 +1449,7 @@
       <c r="K5" s="46"/>
       <c r="L5" s="46"/>
       <c r="M5" s="79" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N5" s="79"/>
       <c r="O5" s="79"/>
@@ -1457,7 +1457,7 @@
       <c r="Q5" s="79"/>
       <c r="R5" s="80"/>
       <c r="S5" s="88" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="T5" s="89"/>
       <c r="U5" s="89"/>
@@ -1478,7 +1478,7 @@
       <c r="K6" s="87"/>
       <c r="L6" s="46"/>
       <c r="M6" s="84" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N6" s="84"/>
       <c r="O6" s="22"/>
@@ -1491,10 +1491,10 @@
       <c r="T6" s="57"/>
       <c r="U6" s="57"/>
       <c r="X6" s="53" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y6" s="1" t="b">
-        <f>AND(COUNTA(K8:K31)&gt;0,COUNTA(J8:J31)=COUNTA(K8:K31))</f>
+        <f>AND(COUNTA(K8:K71)&gt;0,COUNTA(J8:J71)=COUNTA(K8:K71))</f>
         <v>0</v>
       </c>
     </row>
@@ -1513,14 +1513,14 @@
         <v>1</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>2</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="76" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J7" s="22" t="s">
         <v>10</v>
@@ -1558,7 +1558,7 @@
         <v>36</v>
       </c>
       <c r="Y7" s="1">
-        <f>IF(Y6,IF(LARGE($S$8:$S$31,1)&gt;0,LARGE($S$8:$S$31,1),-1),-2)</f>
+        <f>IF(Y6,IF(LARGE($S$8:$S$71,1)&gt;0,LARGE($S$8:$S$71,1),-1),-2)</f>
         <v>-2</v>
       </c>
     </row>
@@ -1567,27 +1567,27 @@
         <v>1</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C8" s="49"/>
       <c r="D8" s="17">
         <v>100001</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F8" s="17">
         <v>1000</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H8" s="13"/>
       <c r="I8" s="20"/>
       <c r="J8" s="23"/>
       <c r="K8" s="23"/>
       <c r="L8" s="23" t="str">
-        <f t="shared" ref="L8:L31" si="0">IF(J8&lt;&gt;"",J8+K8,"")</f>
+        <f t="shared" ref="L8:L39" si="0">IF(J8&lt;&gt;"",J8+K8,"")</f>
         <v/>
       </c>
       <c r="M8" s="23"/>
@@ -1596,11 +1596,11 @@
       <c r="P8" s="13"/>
       <c r="Q8" s="13"/>
       <c r="R8" s="50" t="str">
-        <f>IF(S8=$Y$7,"Bondskampioen",IF(S8=$Y$8,"2e plaats",IF(S8=$Y$9,"3e plaats","")))</f>
+        <f t="shared" ref="R8:R39" si="1">IF(S8=$Y$7,"Bondskampioen",IF(S8=$Y$8,"2e plaats",IF(S8=$Y$9,"3e plaats","")))</f>
         <v/>
       </c>
       <c r="S8" s="13">
-        <f t="shared" ref="S8:S31" si="1">IF(L8&lt;&gt;"", L8+M8/100+N8/10000+O8/1000000,0)</f>
+        <f t="shared" ref="S8:S39" si="2">IF(L8&lt;&gt;"", L8+M8/100+N8/10000+O8/1000000,0)</f>
         <v>0</v>
       </c>
       <c r="T8" s="2"/>
@@ -1611,11 +1611,12 @@
         <v>37</v>
       </c>
       <c r="Y8" s="1">
-        <f>IF(Y6,IF(LARGE($S$8:$S$31,2)&gt;0,LARGE($S$8:$S$31,2),-1),-2)</f>
+        <f>IF(Y6,IF(LARGE($S$8:$S$71,2)&gt;0,LARGE($S$8:$S$71,2),-1),-2)</f>
         <v>-2</v>
       </c>
     </row>
     <row r="9" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="53"/>
       <c r="C9" s="49"/>
       <c r="D9" s="17"/>
       <c r="E9" s="13"/>
@@ -1635,11 +1636,11 @@
       <c r="P9" s="13"/>
       <c r="Q9" s="13"/>
       <c r="R9" s="50" t="str">
-        <f t="shared" ref="R9:R31" si="2">IF(S9=$Y$7,"Bondskampioen",IF(S9=$Y$8,"2e plaats",IF(S9=$Y$9,"3e plaats","")))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S9" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T9" s="12"/>
@@ -1650,12 +1651,12 @@
         <v>38</v>
       </c>
       <c r="Y9" s="1">
-        <f>IF(Y6,IF(LARGE($S$8:$S$31,3)&gt;0,LARGE($S$8:$S$31,3),-1),-2)</f>
+        <f>IF(Y6,IF(LARGE($S$8:$S$71,3)&gt;0,LARGE($S$8:$S$71,3),-1),-2)</f>
         <v>-2</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A10" s="18"/>
+      <c r="A10" s="53"/>
       <c r="B10" s="18"/>
       <c r="C10" s="49"/>
       <c r="D10" s="17"/>
@@ -1676,11 +1677,11 @@
       <c r="P10" s="13"/>
       <c r="Q10" s="13"/>
       <c r="R10" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S10" s="13">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="S10" s="13">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T10" s="12"/>
@@ -1689,7 +1690,7 @@
       <c r="W10"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A11" s="18"/>
+      <c r="A11" s="53"/>
       <c r="B11" s="18"/>
       <c r="C11" s="49"/>
       <c r="D11" s="17"/>
@@ -1710,11 +1711,11 @@
       <c r="P11" s="13"/>
       <c r="Q11" s="13"/>
       <c r="R11" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S11" s="13">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="S11" s="13">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T11" s="2"/>
@@ -1723,7 +1724,7 @@
       <c r="W11"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A12" s="18"/>
+      <c r="A12" s="53"/>
       <c r="B12" s="18"/>
       <c r="C12" s="49"/>
       <c r="D12" s="17"/>
@@ -1744,11 +1745,11 @@
       <c r="P12" s="13"/>
       <c r="Q12" s="13"/>
       <c r="R12" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S12" s="13">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="S12" s="13">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T12" s="2"/>
@@ -1757,7 +1758,7 @@
       <c r="W12"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A13" s="18"/>
+      <c r="A13" s="53"/>
       <c r="B13" s="18"/>
       <c r="C13" s="49"/>
       <c r="D13" s="17"/>
@@ -1778,11 +1779,11 @@
       <c r="P13" s="13"/>
       <c r="Q13" s="13"/>
       <c r="R13" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S13" s="13">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="S13" s="13">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T13" s="2"/>
@@ -1791,7 +1792,7 @@
       <c r="W13"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A14" s="18"/>
+      <c r="A14" s="53"/>
       <c r="B14" s="18"/>
       <c r="C14" s="49"/>
       <c r="D14" s="17"/>
@@ -1812,11 +1813,11 @@
       <c r="P14" s="13"/>
       <c r="Q14" s="13"/>
       <c r="R14" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S14" s="13">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="S14" s="13">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T14" s="2"/>
@@ -1825,7 +1826,7 @@
       <c r="W14"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A15" s="18"/>
+      <c r="A15" s="53"/>
       <c r="B15" s="18"/>
       <c r="C15" s="49"/>
       <c r="D15" s="17"/>
@@ -1846,11 +1847,11 @@
       <c r="P15" s="13"/>
       <c r="Q15" s="13"/>
       <c r="R15" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S15" s="13">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="S15" s="13">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T15" s="2"/>
@@ -1859,7 +1860,7 @@
       <c r="W15"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A16" s="18"/>
+      <c r="A16" s="53"/>
       <c r="B16" s="18"/>
       <c r="C16" s="49"/>
       <c r="D16" s="17"/>
@@ -1880,11 +1881,11 @@
       <c r="P16" s="13"/>
       <c r="Q16" s="13"/>
       <c r="R16" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S16" s="13">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="S16" s="13">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T16" s="2"/>
@@ -1893,7 +1894,7 @@
       <c r="W16"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A17" s="18"/>
+      <c r="A17" s="53"/>
       <c r="B17" s="18"/>
       <c r="C17" s="49"/>
       <c r="D17" s="17"/>
@@ -1914,11 +1915,11 @@
       <c r="P17" s="13"/>
       <c r="Q17" s="13"/>
       <c r="R17" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S17" s="13">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="S17" s="13">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T17" s="2"/>
@@ -1927,7 +1928,7 @@
       <c r="W17"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A18" s="18"/>
+      <c r="A18" s="53"/>
       <c r="B18" s="18"/>
       <c r="C18" s="49"/>
       <c r="D18" s="17"/>
@@ -1948,11 +1949,11 @@
       <c r="P18" s="13"/>
       <c r="Q18" s="13"/>
       <c r="R18" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S18" s="13">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="S18" s="13">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T18" s="2"/>
@@ -1961,7 +1962,7 @@
       <c r="W18"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A19" s="18"/>
+      <c r="A19" s="53"/>
       <c r="B19" s="18"/>
       <c r="C19" s="49"/>
       <c r="D19" s="17"/>
@@ -1982,11 +1983,11 @@
       <c r="P19" s="13"/>
       <c r="Q19" s="13"/>
       <c r="R19" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S19" s="13">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="S19" s="13">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T19" s="2"/>
@@ -1995,7 +1996,7 @@
       <c r="W19"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A20" s="18"/>
+      <c r="A20" s="53"/>
       <c r="B20" s="18"/>
       <c r="C20" s="49"/>
       <c r="D20" s="17"/>
@@ -2016,11 +2017,11 @@
       <c r="P20" s="13"/>
       <c r="Q20" s="13"/>
       <c r="R20" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S20" s="13">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="S20" s="13">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T20" s="2"/>
@@ -2029,7 +2030,7 @@
       <c r="W20"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A21" s="18"/>
+      <c r="A21" s="53"/>
       <c r="B21" s="18"/>
       <c r="C21" s="49"/>
       <c r="D21" s="17"/>
@@ -2050,11 +2051,11 @@
       <c r="P21" s="13"/>
       <c r="Q21" s="13"/>
       <c r="R21" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S21" s="13">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="S21" s="13">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T21" s="2"/>
@@ -2063,7 +2064,7 @@
       <c r="W21"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A22" s="18"/>
+      <c r="A22" s="53"/>
       <c r="B22" s="18"/>
       <c r="C22" s="49"/>
       <c r="D22" s="17"/>
@@ -2084,11 +2085,11 @@
       <c r="P22" s="13"/>
       <c r="Q22" s="13"/>
       <c r="R22" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S22" s="13">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="S22" s="13">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T22" s="2"/>
@@ -2097,7 +2098,7 @@
       <c r="W22"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A23" s="18"/>
+      <c r="A23" s="53"/>
       <c r="B23" s="18"/>
       <c r="C23" s="49"/>
       <c r="D23" s="17"/>
@@ -2118,11 +2119,11 @@
       <c r="P23" s="13"/>
       <c r="Q23" s="13"/>
       <c r="R23" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S23" s="13">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="S23" s="13">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T23" s="2"/>
@@ -2131,32 +2132,32 @@
       <c r="W23"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A24" s="18"/>
+      <c r="A24" s="53"/>
       <c r="B24" s="3"/>
       <c r="C24" s="49"/>
-      <c r="D24" s="15"/>
+      <c r="D24" s="17"/>
       <c r="E24"/>
       <c r="F24" s="16"/>
       <c r="G24" s="16"/>
       <c r="H24"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="21"/>
-      <c r="K24" s="21"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
       <c r="L24" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M24" s="21"/>
-      <c r="N24" s="21"/>
-      <c r="O24" s="21"/>
-      <c r="P24"/>
-      <c r="Q24"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="13"/>
       <c r="R24" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S24" s="13">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="S24" s="13">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T24" s="2"/>
@@ -2165,32 +2166,32 @@
       <c r="W24"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A25" s="18"/>
+      <c r="A25" s="53"/>
       <c r="B25" s="3"/>
       <c r="C25" s="49"/>
-      <c r="D25" s="15"/>
+      <c r="D25" s="17"/>
       <c r="E25"/>
       <c r="F25" s="16"/>
       <c r="G25" s="16"/>
       <c r="H25"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="23"/>
       <c r="L25" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M25" s="21"/>
-      <c r="N25" s="21"/>
-      <c r="O25" s="21"/>
-      <c r="P25"/>
-      <c r="Q25"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="13"/>
       <c r="R25" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S25" s="13">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="S25" s="13">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T25" s="2"/>
@@ -2199,32 +2200,32 @@
       <c r="W25"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A26" s="18"/>
+      <c r="A26" s="53"/>
       <c r="B26" s="3"/>
       <c r="C26" s="49"/>
-      <c r="D26" s="15"/>
+      <c r="D26" s="17"/>
       <c r="E26"/>
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
       <c r="H26"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="21"/>
-      <c r="K26" s="21"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="23"/>
       <c r="L26" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M26" s="21"/>
-      <c r="N26" s="21"/>
-      <c r="O26" s="21"/>
-      <c r="P26"/>
-      <c r="Q26"/>
+      <c r="M26" s="23"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="23"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="13"/>
       <c r="R26" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S26" s="13">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="S26" s="13">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T26" s="2"/>
@@ -2233,32 +2234,32 @@
       <c r="W26"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A27" s="18"/>
+      <c r="A27" s="53"/>
       <c r="B27" s="3"/>
       <c r="C27" s="49"/>
-      <c r="D27" s="15"/>
+      <c r="D27" s="17"/>
       <c r="E27"/>
       <c r="F27" s="16"/>
       <c r="G27" s="16"/>
       <c r="H27"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="21"/>
-      <c r="K27" s="21"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
       <c r="L27" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M27" s="21"/>
-      <c r="N27" s="21"/>
-      <c r="O27" s="21"/>
-      <c r="P27"/>
-      <c r="Q27"/>
+      <c r="M27" s="23"/>
+      <c r="N27" s="23"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
       <c r="R27" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S27" s="13">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="S27" s="13">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T27" s="2"/>
@@ -2267,32 +2268,32 @@
       <c r="W27"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A28" s="18"/>
+      <c r="A28" s="53"/>
       <c r="B28" s="3"/>
       <c r="C28" s="49"/>
-      <c r="D28" s="15"/>
+      <c r="D28" s="17"/>
       <c r="E28"/>
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
       <c r="H28"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="21"/>
-      <c r="K28" s="21"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
       <c r="L28" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M28" s="21"/>
-      <c r="N28" s="21"/>
-      <c r="O28" s="21"/>
-      <c r="P28"/>
-      <c r="Q28"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="23"/>
+      <c r="O28" s="23"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="13"/>
       <c r="R28" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S28" s="13">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="S28" s="13">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T28" s="2"/>
@@ -2301,32 +2302,32 @@
       <c r="W28"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A29" s="18"/>
+      <c r="A29" s="53"/>
       <c r="B29" s="3"/>
       <c r="C29" s="49"/>
-      <c r="D29" s="15"/>
+      <c r="D29" s="17"/>
       <c r="E29"/>
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
       <c r="H29"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="21"/>
-      <c r="K29" s="21"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
       <c r="L29" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M29" s="21"/>
-      <c r="N29" s="21"/>
-      <c r="O29" s="21"/>
-      <c r="P29"/>
-      <c r="Q29"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23"/>
+      <c r="O29" s="23"/>
+      <c r="P29" s="13"/>
+      <c r="Q29" s="13"/>
       <c r="R29" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S29" s="13">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="S29" s="13">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T29" s="2"/>
@@ -2335,32 +2336,32 @@
       <c r="W29"/>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A30" s="18"/>
+      <c r="A30" s="53"/>
       <c r="B30" s="3"/>
       <c r="C30" s="49"/>
-      <c r="D30" s="15"/>
+      <c r="D30" s="17"/>
       <c r="E30"/>
       <c r="F30" s="16"/>
       <c r="G30" s="16"/>
       <c r="H30"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="21"/>
-      <c r="K30" s="21"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="23"/>
       <c r="L30" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M30" s="21"/>
-      <c r="N30" s="21"/>
-      <c r="O30" s="21"/>
-      <c r="P30"/>
-      <c r="Q30"/>
+      <c r="M30" s="23"/>
+      <c r="N30" s="23"/>
+      <c r="O30" s="23"/>
+      <c r="P30" s="13"/>
+      <c r="Q30" s="13"/>
       <c r="R30" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S30" s="13">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="S30" s="13">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T30" s="2"/>
@@ -2368,228 +2369,1543 @@
       <c r="V30"/>
       <c r="W30"/>
     </row>
-    <row r="31" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
-      <c r="B31" s="3"/>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A31" s="53"/>
+      <c r="B31" s="18"/>
       <c r="C31" s="49"/>
-      <c r="D31" s="15"/>
-      <c r="E31"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="21"/>
-      <c r="K31" s="21"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="23"/>
+      <c r="K31" s="23"/>
       <c r="L31" s="23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M31" s="21"/>
-      <c r="N31" s="21"/>
-      <c r="O31" s="21"/>
-      <c r="P31"/>
-      <c r="Q31"/>
+      <c r="M31" s="23"/>
+      <c r="N31" s="23"/>
+      <c r="O31" s="23"/>
+      <c r="P31" s="13"/>
+      <c r="Q31" s="13"/>
       <c r="R31" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S31" s="13">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="S31" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T31" s="2"/>
-      <c r="U31" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="T31" s="12"/>
+      <c r="U31" s="12"/>
       <c r="V31"/>
       <c r="W31"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A32" s="58"/>
-      <c r="B32" s="58"/>
-      <c r="C32" s="59"/>
-      <c r="D32" s="60"/>
-      <c r="E32" s="61"/>
-      <c r="F32" s="62"/>
-      <c r="G32" s="62"/>
-      <c r="H32" s="61"/>
-      <c r="I32" s="63"/>
-      <c r="J32" s="64"/>
-      <c r="K32" s="64"/>
-      <c r="L32" s="65"/>
-      <c r="M32" s="64"/>
-      <c r="N32" s="64"/>
-      <c r="O32" s="64"/>
-      <c r="P32" s="61"/>
-      <c r="Q32" s="61"/>
-      <c r="R32" s="61"/>
-      <c r="S32" s="39"/>
-      <c r="T32" s="38"/>
-      <c r="U32" s="38"/>
+      <c r="A32" s="53"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M32" s="23"/>
+      <c r="N32" s="23"/>
+      <c r="O32" s="23"/>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="13"/>
+      <c r="R32" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S32" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2"/>
       <c r="V32"/>
       <c r="W32"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A33" s="56" t="s">
-        <v>12</v>
-      </c>
-      <c r="B33" s="40"/>
-      <c r="C33" s="39"/>
-      <c r="D33" s="66"/>
-      <c r="E33" s="39"/>
-      <c r="F33" s="71"/>
-      <c r="G33" s="67" t="s">
-        <v>42</v>
-      </c>
-      <c r="H33" s="39"/>
-      <c r="I33" s="68"/>
-      <c r="J33" s="41"/>
-      <c r="K33" s="41"/>
-      <c r="L33" s="69" t="s">
-        <v>39</v>
-      </c>
-      <c r="M33" s="41"/>
-      <c r="N33" s="41"/>
-      <c r="O33" s="41"/>
-      <c r="P33" s="39"/>
-      <c r="Q33" s="39"/>
-      <c r="R33" s="70" t="s">
-        <v>39</v>
-      </c>
-      <c r="S33" s="70" t="s">
-        <v>39</v>
-      </c>
-      <c r="T33" s="38"/>
-      <c r="U33" s="38"/>
+      <c r="A33" s="53"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="23"/>
+      <c r="L33" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M33" s="23"/>
+      <c r="N33" s="23"/>
+      <c r="O33" s="23"/>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="13"/>
+      <c r="R33" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S33" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
       <c r="V33"/>
       <c r="W33"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A34" s="58"/>
-      <c r="B34" s="58"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="66"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="71"/>
-      <c r="G34" s="71"/>
-      <c r="H34" s="39"/>
-      <c r="I34" s="68"/>
-      <c r="J34" s="41"/>
-      <c r="K34" s="41"/>
-      <c r="L34" s="69" t="s">
-        <v>39</v>
-      </c>
-      <c r="M34" s="72"/>
-      <c r="N34" s="72"/>
-      <c r="O34" s="72"/>
-      <c r="P34" s="73"/>
-      <c r="Q34" s="73"/>
-      <c r="R34" s="70" t="s">
-        <v>39</v>
-      </c>
-      <c r="S34" s="70" t="s">
-        <v>39</v>
-      </c>
-      <c r="T34" s="38"/>
-      <c r="U34" s="38"/>
+      <c r="A34" s="53"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="23"/>
+      <c r="K34" s="23"/>
+      <c r="L34" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M34" s="23"/>
+      <c r="N34" s="23"/>
+      <c r="O34" s="23"/>
+      <c r="P34" s="13"/>
+      <c r="Q34" s="13"/>
+      <c r="R34" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S34" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2"/>
       <c r="V34"/>
       <c r="W34"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A35" s="56" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35" s="40"/>
-      <c r="C35" s="39"/>
-      <c r="D35" s="74"/>
-      <c r="E35" s="39"/>
-      <c r="F35" s="71"/>
-      <c r="G35" s="71"/>
-      <c r="H35" s="39"/>
-      <c r="I35" s="68"/>
-      <c r="J35" s="41"/>
-      <c r="K35" s="41"/>
-      <c r="L35" s="78" t="s">
-        <v>40</v>
-      </c>
-      <c r="M35" s="78"/>
-      <c r="N35" s="78"/>
-      <c r="O35" s="78"/>
-      <c r="P35" s="78"/>
-      <c r="Q35" s="78"/>
-      <c r="R35" s="78"/>
-      <c r="S35" s="78"/>
-      <c r="T35" s="38"/>
-      <c r="U35" s="38"/>
+      <c r="A35" s="53"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="23"/>
+      <c r="K35" s="23"/>
+      <c r="L35" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M35" s="23"/>
+      <c r="N35" s="23"/>
+      <c r="O35" s="23"/>
+      <c r="P35" s="13"/>
+      <c r="Q35" s="13"/>
+      <c r="R35" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S35" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
       <c r="V35"/>
       <c r="W35"/>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="D36" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E36" s="7" t="s">
+      <c r="A36" s="53"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="23"/>
+      <c r="K36" s="23"/>
+      <c r="L36" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M36" s="23"/>
+      <c r="N36" s="23"/>
+      <c r="O36" s="23"/>
+      <c r="P36" s="13"/>
+      <c r="Q36" s="13"/>
+      <c r="R36" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S36" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T36" s="2"/>
+      <c r="U36" s="2"/>
+      <c r="V36"/>
+      <c r="W36"/>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A37" s="53"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="23"/>
+      <c r="K37" s="23"/>
+      <c r="L37" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M37" s="23"/>
+      <c r="N37" s="23"/>
+      <c r="O37" s="23"/>
+      <c r="P37" s="13"/>
+      <c r="Q37" s="13"/>
+      <c r="R37" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S37" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T37" s="2"/>
+      <c r="U37" s="2"/>
+      <c r="V37"/>
+      <c r="W37"/>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A38" s="53"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="23"/>
+      <c r="K38" s="23"/>
+      <c r="L38" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M38" s="23"/>
+      <c r="N38" s="23"/>
+      <c r="O38" s="23"/>
+      <c r="P38" s="13"/>
+      <c r="Q38" s="13"/>
+      <c r="R38" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S38" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T38" s="2"/>
+      <c r="U38" s="2"/>
+      <c r="V38"/>
+      <c r="W38"/>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A39" s="53"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="23"/>
+      <c r="K39" s="23"/>
+      <c r="L39" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="M39" s="23"/>
+      <c r="N39" s="23"/>
+      <c r="O39" s="23"/>
+      <c r="P39" s="13"/>
+      <c r="Q39" s="13"/>
+      <c r="R39" s="50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S39" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T39" s="2"/>
+      <c r="U39" s="2"/>
+      <c r="V39"/>
+      <c r="W39"/>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A40" s="53"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="23"/>
+      <c r="K40" s="23"/>
+      <c r="L40" s="23" t="str">
+        <f t="shared" ref="L40:L71" si="3">IF(J40&lt;&gt;"",J40+K40,"")</f>
+        <v/>
+      </c>
+      <c r="M40" s="23"/>
+      <c r="N40" s="23"/>
+      <c r="O40" s="23"/>
+      <c r="P40" s="13"/>
+      <c r="Q40" s="13"/>
+      <c r="R40" s="50" t="str">
+        <f t="shared" ref="R40:R71" si="4">IF(S40=$Y$7,"Bondskampioen",IF(S40=$Y$8,"2e plaats",IF(S40=$Y$9,"3e plaats","")))</f>
+        <v/>
+      </c>
+      <c r="S40" s="13">
+        <f t="shared" ref="S40:S71" si="5">IF(L40&lt;&gt;"", L40+M40/100+N40/10000+O40/1000000,0)</f>
+        <v>0</v>
+      </c>
+      <c r="T40" s="2"/>
+      <c r="U40" s="2"/>
+      <c r="V40"/>
+      <c r="W40"/>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A41" s="53"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="49"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="20"/>
+      <c r="J41" s="23"/>
+      <c r="K41" s="23"/>
+      <c r="L41" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M41" s="23"/>
+      <c r="N41" s="23"/>
+      <c r="O41" s="23"/>
+      <c r="P41" s="13"/>
+      <c r="Q41" s="13"/>
+      <c r="R41" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S41" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T41" s="2"/>
+      <c r="U41" s="2"/>
+      <c r="V41"/>
+      <c r="W41"/>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A42" s="53"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="23"/>
+      <c r="K42" s="23"/>
+      <c r="L42" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M42" s="23"/>
+      <c r="N42" s="23"/>
+      <c r="O42" s="23"/>
+      <c r="P42" s="13"/>
+      <c r="Q42" s="13"/>
+      <c r="R42" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S42" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T42" s="2"/>
+      <c r="U42" s="2"/>
+      <c r="V42"/>
+      <c r="W42"/>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A43" s="53"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="49"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="23"/>
+      <c r="K43" s="23"/>
+      <c r="L43" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M43" s="23"/>
+      <c r="N43" s="23"/>
+      <c r="O43" s="23"/>
+      <c r="P43" s="13"/>
+      <c r="Q43" s="13"/>
+      <c r="R43" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S43" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T43" s="2"/>
+      <c r="U43" s="2"/>
+      <c r="V43"/>
+      <c r="W43"/>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A44" s="53"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="49"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="23"/>
+      <c r="K44" s="23"/>
+      <c r="L44" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M44" s="23"/>
+      <c r="N44" s="23"/>
+      <c r="O44" s="23"/>
+      <c r="P44" s="13"/>
+      <c r="Q44" s="13"/>
+      <c r="R44" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S44" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T44" s="2"/>
+      <c r="U44" s="2"/>
+      <c r="V44"/>
+      <c r="W44"/>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A45" s="53"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="49"/>
+      <c r="D45" s="17"/>
+      <c r="E45"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45"/>
+      <c r="I45" s="20"/>
+      <c r="J45" s="23"/>
+      <c r="K45" s="23"/>
+      <c r="L45" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M45" s="23"/>
+      <c r="N45" s="23"/>
+      <c r="O45" s="23"/>
+      <c r="P45" s="13"/>
+      <c r="Q45" s="13"/>
+      <c r="R45" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S45" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T45" s="2"/>
+      <c r="U45" s="2"/>
+      <c r="V45"/>
+      <c r="W45"/>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A46" s="53"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="49"/>
+      <c r="D46" s="17"/>
+      <c r="E46"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46"/>
+      <c r="I46" s="20"/>
+      <c r="J46" s="23"/>
+      <c r="K46" s="23"/>
+      <c r="L46" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M46" s="23"/>
+      <c r="N46" s="23"/>
+      <c r="O46" s="23"/>
+      <c r="P46" s="13"/>
+      <c r="Q46" s="13"/>
+      <c r="R46" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S46" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T46" s="2"/>
+      <c r="U46" s="2"/>
+      <c r="V46"/>
+      <c r="W46"/>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A47" s="53"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="49"/>
+      <c r="D47" s="17"/>
+      <c r="E47"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47"/>
+      <c r="I47" s="20"/>
+      <c r="J47" s="23"/>
+      <c r="K47" s="23"/>
+      <c r="L47" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M47" s="23"/>
+      <c r="N47" s="23"/>
+      <c r="O47" s="23"/>
+      <c r="P47" s="13"/>
+      <c r="Q47" s="13"/>
+      <c r="R47" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S47" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T47" s="2"/>
+      <c r="U47" s="2"/>
+      <c r="V47"/>
+      <c r="W47"/>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A48" s="53"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="49"/>
+      <c r="D48" s="17"/>
+      <c r="E48"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
+      <c r="H48"/>
+      <c r="I48" s="20"/>
+      <c r="J48" s="23"/>
+      <c r="K48" s="23"/>
+      <c r="L48" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M48" s="23"/>
+      <c r="N48" s="23"/>
+      <c r="O48" s="23"/>
+      <c r="P48" s="13"/>
+      <c r="Q48" s="13"/>
+      <c r="R48" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S48" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T48" s="2"/>
+      <c r="U48" s="2"/>
+      <c r="V48"/>
+      <c r="W48"/>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A49" s="53"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="49"/>
+      <c r="D49" s="17"/>
+      <c r="E49"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="16"/>
+      <c r="H49"/>
+      <c r="I49" s="20"/>
+      <c r="J49" s="23"/>
+      <c r="K49" s="23"/>
+      <c r="L49" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M49" s="23"/>
+      <c r="N49" s="23"/>
+      <c r="O49" s="23"/>
+      <c r="P49" s="13"/>
+      <c r="Q49" s="13"/>
+      <c r="R49" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S49" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T49" s="2"/>
+      <c r="U49" s="2"/>
+      <c r="V49"/>
+      <c r="W49"/>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A50" s="53"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="49"/>
+      <c r="D50" s="17"/>
+      <c r="E50"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="16"/>
+      <c r="H50"/>
+      <c r="I50" s="20"/>
+      <c r="J50" s="23"/>
+      <c r="K50" s="23"/>
+      <c r="L50" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M50" s="23"/>
+      <c r="N50" s="23"/>
+      <c r="O50" s="23"/>
+      <c r="P50" s="13"/>
+      <c r="Q50" s="13"/>
+      <c r="R50" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S50" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T50" s="2"/>
+      <c r="U50" s="2"/>
+      <c r="V50"/>
+      <c r="W50"/>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A51" s="53"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="49"/>
+      <c r="D51" s="17"/>
+      <c r="E51"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="16"/>
+      <c r="H51"/>
+      <c r="I51" s="20"/>
+      <c r="J51" s="23"/>
+      <c r="K51" s="23"/>
+      <c r="L51" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M51" s="23"/>
+      <c r="N51" s="23"/>
+      <c r="O51" s="23"/>
+      <c r="P51" s="13"/>
+      <c r="Q51" s="13"/>
+      <c r="R51" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S51" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T51" s="2"/>
+      <c r="U51" s="2"/>
+      <c r="V51"/>
+      <c r="W51"/>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A52" s="53"/>
+      <c r="B52" s="18"/>
+      <c r="C52" s="49"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="19"/>
+      <c r="G52" s="19"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="20"/>
+      <c r="J52" s="23"/>
+      <c r="K52" s="23"/>
+      <c r="L52" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M52" s="23"/>
+      <c r="N52" s="23"/>
+      <c r="O52" s="23"/>
+      <c r="P52" s="13"/>
+      <c r="Q52" s="13"/>
+      <c r="R52" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S52" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T52" s="12"/>
+      <c r="U52" s="12"/>
+      <c r="V52"/>
+      <c r="W52"/>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A53" s="53"/>
+      <c r="B53" s="18"/>
+      <c r="C53" s="49"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="19"/>
+      <c r="G53" s="19"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="20"/>
+      <c r="J53" s="23"/>
+      <c r="K53" s="23"/>
+      <c r="L53" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M53" s="23"/>
+      <c r="N53" s="23"/>
+      <c r="O53" s="23"/>
+      <c r="P53" s="13"/>
+      <c r="Q53" s="13"/>
+      <c r="R53" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S53" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T53" s="2"/>
+      <c r="U53" s="2"/>
+      <c r="V53"/>
+      <c r="W53"/>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A54" s="53"/>
+      <c r="B54" s="18"/>
+      <c r="C54" s="49"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="19"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="13"/>
+      <c r="I54" s="20"/>
+      <c r="J54" s="23"/>
+      <c r="K54" s="23"/>
+      <c r="L54" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M54" s="23"/>
+      <c r="N54" s="23"/>
+      <c r="O54" s="23"/>
+      <c r="P54" s="13"/>
+      <c r="Q54" s="13"/>
+      <c r="R54" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S54" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T54" s="2"/>
+      <c r="U54" s="2"/>
+      <c r="V54"/>
+      <c r="W54"/>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A55" s="53"/>
+      <c r="B55" s="18"/>
+      <c r="C55" s="49"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="19"/>
+      <c r="G55" s="19"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="20"/>
+      <c r="J55" s="23"/>
+      <c r="K55" s="23"/>
+      <c r="L55" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M55" s="23"/>
+      <c r="N55" s="23"/>
+      <c r="O55" s="23"/>
+      <c r="P55" s="13"/>
+      <c r="Q55" s="13"/>
+      <c r="R55" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S55" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T55" s="2"/>
+      <c r="U55" s="2"/>
+      <c r="V55"/>
+      <c r="W55"/>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A56" s="53"/>
+      <c r="B56" s="18"/>
+      <c r="C56" s="49"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="19"/>
+      <c r="G56" s="19"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="20"/>
+      <c r="J56" s="23"/>
+      <c r="K56" s="23"/>
+      <c r="L56" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M56" s="23"/>
+      <c r="N56" s="23"/>
+      <c r="O56" s="23"/>
+      <c r="P56" s="13"/>
+      <c r="Q56" s="13"/>
+      <c r="R56" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S56" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T56" s="2"/>
+      <c r="U56" s="2"/>
+      <c r="V56"/>
+      <c r="W56"/>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A57" s="53"/>
+      <c r="B57" s="18"/>
+      <c r="C57" s="49"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="19"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="20"/>
+      <c r="J57" s="23"/>
+      <c r="K57" s="23"/>
+      <c r="L57" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M57" s="23"/>
+      <c r="N57" s="23"/>
+      <c r="O57" s="23"/>
+      <c r="P57" s="13"/>
+      <c r="Q57" s="13"/>
+      <c r="R57" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S57" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T57" s="2"/>
+      <c r="U57" s="2"/>
+      <c r="V57"/>
+      <c r="W57"/>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A58" s="53"/>
+      <c r="B58" s="18"/>
+      <c r="C58" s="49"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="19"/>
+      <c r="G58" s="19"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="20"/>
+      <c r="J58" s="23"/>
+      <c r="K58" s="23"/>
+      <c r="L58" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M58" s="23"/>
+      <c r="N58" s="23"/>
+      <c r="O58" s="23"/>
+      <c r="P58" s="13"/>
+      <c r="Q58" s="13"/>
+      <c r="R58" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S58" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T58" s="2"/>
+      <c r="U58" s="2"/>
+      <c r="V58"/>
+      <c r="W58"/>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A59" s="53"/>
+      <c r="B59" s="18"/>
+      <c r="C59" s="49"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="19"/>
+      <c r="G59" s="19"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="20"/>
+      <c r="J59" s="23"/>
+      <c r="K59" s="23"/>
+      <c r="L59" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M59" s="23"/>
+      <c r="N59" s="23"/>
+      <c r="O59" s="23"/>
+      <c r="P59" s="13"/>
+      <c r="Q59" s="13"/>
+      <c r="R59" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S59" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T59" s="2"/>
+      <c r="U59" s="2"/>
+      <c r="V59"/>
+      <c r="W59"/>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A60" s="53"/>
+      <c r="B60" s="18"/>
+      <c r="C60" s="49"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="19"/>
+      <c r="G60" s="19"/>
+      <c r="H60" s="13"/>
+      <c r="I60" s="20"/>
+      <c r="J60" s="23"/>
+      <c r="K60" s="23"/>
+      <c r="L60" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M60" s="23"/>
+      <c r="N60" s="23"/>
+      <c r="O60" s="23"/>
+      <c r="P60" s="13"/>
+      <c r="Q60" s="13"/>
+      <c r="R60" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S60" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T60" s="2"/>
+      <c r="U60" s="2"/>
+      <c r="V60"/>
+      <c r="W60"/>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A61" s="53"/>
+      <c r="B61" s="18"/>
+      <c r="C61" s="49"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="19"/>
+      <c r="G61" s="19"/>
+      <c r="H61" s="13"/>
+      <c r="I61" s="20"/>
+      <c r="J61" s="23"/>
+      <c r="K61" s="23"/>
+      <c r="L61" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M61" s="23"/>
+      <c r="N61" s="23"/>
+      <c r="O61" s="23"/>
+      <c r="P61" s="13"/>
+      <c r="Q61" s="13"/>
+      <c r="R61" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S61" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T61" s="2"/>
+      <c r="U61" s="2"/>
+      <c r="V61"/>
+      <c r="W61"/>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A62" s="53"/>
+      <c r="B62" s="18"/>
+      <c r="C62" s="49"/>
+      <c r="D62" s="17"/>
+      <c r="E62" s="13"/>
+      <c r="F62" s="19"/>
+      <c r="G62" s="19"/>
+      <c r="H62" s="13"/>
+      <c r="I62" s="20"/>
+      <c r="J62" s="23"/>
+      <c r="K62" s="23"/>
+      <c r="L62" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M62" s="23"/>
+      <c r="N62" s="23"/>
+      <c r="O62" s="23"/>
+      <c r="P62" s="13"/>
+      <c r="Q62" s="13"/>
+      <c r="R62" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S62" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T62" s="2"/>
+      <c r="U62" s="2"/>
+      <c r="V62"/>
+      <c r="W62"/>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A63" s="53"/>
+      <c r="B63" s="18"/>
+      <c r="C63" s="49"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="19"/>
+      <c r="G63" s="19"/>
+      <c r="H63" s="13"/>
+      <c r="I63" s="20"/>
+      <c r="J63" s="23"/>
+      <c r="K63" s="23"/>
+      <c r="L63" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M63" s="23"/>
+      <c r="N63" s="23"/>
+      <c r="O63" s="23"/>
+      <c r="P63" s="13"/>
+      <c r="Q63" s="13"/>
+      <c r="R63" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S63" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T63" s="2"/>
+      <c r="U63" s="2"/>
+      <c r="V63"/>
+      <c r="W63"/>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A64" s="53"/>
+      <c r="B64" s="18"/>
+      <c r="C64" s="49"/>
+      <c r="D64" s="17"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="19"/>
+      <c r="G64" s="19"/>
+      <c r="H64" s="13"/>
+      <c r="I64" s="20"/>
+      <c r="J64" s="23"/>
+      <c r="K64" s="23"/>
+      <c r="L64" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M64" s="23"/>
+      <c r="N64" s="23"/>
+      <c r="O64" s="23"/>
+      <c r="P64" s="13"/>
+      <c r="Q64" s="13"/>
+      <c r="R64" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S64" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T64" s="2"/>
+      <c r="U64" s="2"/>
+      <c r="V64"/>
+      <c r="W64"/>
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A65" s="53"/>
+      <c r="B65" s="18"/>
+      <c r="C65" s="49"/>
+      <c r="D65" s="17"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="19"/>
+      <c r="G65" s="19"/>
+      <c r="H65" s="13"/>
+      <c r="I65" s="20"/>
+      <c r="J65" s="23"/>
+      <c r="K65" s="23"/>
+      <c r="L65" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M65" s="23"/>
+      <c r="N65" s="23"/>
+      <c r="O65" s="23"/>
+      <c r="P65" s="13"/>
+      <c r="Q65" s="13"/>
+      <c r="R65" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S65" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T65" s="2"/>
+      <c r="U65" s="2"/>
+      <c r="V65"/>
+      <c r="W65"/>
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A66" s="53"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="49"/>
+      <c r="D66" s="17"/>
+      <c r="E66"/>
+      <c r="F66" s="16"/>
+      <c r="G66" s="16"/>
+      <c r="H66"/>
+      <c r="I66" s="20"/>
+      <c r="J66" s="23"/>
+      <c r="K66" s="23"/>
+      <c r="L66" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M66" s="23"/>
+      <c r="N66" s="23"/>
+      <c r="O66" s="23"/>
+      <c r="P66" s="13"/>
+      <c r="Q66" s="13"/>
+      <c r="R66" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S66" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T66" s="2"/>
+      <c r="U66" s="2"/>
+      <c r="V66"/>
+      <c r="W66"/>
+    </row>
+    <row r="67" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A67" s="53"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="49"/>
+      <c r="D67" s="17"/>
+      <c r="E67"/>
+      <c r="F67" s="16"/>
+      <c r="G67" s="16"/>
+      <c r="H67"/>
+      <c r="I67" s="20"/>
+      <c r="J67" s="23"/>
+      <c r="K67" s="23"/>
+      <c r="L67" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M67" s="23"/>
+      <c r="N67" s="23"/>
+      <c r="O67" s="23"/>
+      <c r="P67" s="13"/>
+      <c r="Q67" s="13"/>
+      <c r="R67" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S67" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T67" s="2"/>
+      <c r="U67" s="2"/>
+      <c r="V67"/>
+      <c r="W67"/>
+    </row>
+    <row r="68" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A68" s="53"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="49"/>
+      <c r="D68" s="17"/>
+      <c r="E68"/>
+      <c r="F68" s="16"/>
+      <c r="G68" s="16"/>
+      <c r="H68"/>
+      <c r="I68" s="20"/>
+      <c r="J68" s="23"/>
+      <c r="K68" s="23"/>
+      <c r="L68" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M68" s="23"/>
+      <c r="N68" s="23"/>
+      <c r="O68" s="23"/>
+      <c r="P68" s="13"/>
+      <c r="Q68" s="13"/>
+      <c r="R68" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S68" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T68" s="2"/>
+      <c r="U68" s="2"/>
+      <c r="V68"/>
+      <c r="W68"/>
+    </row>
+    <row r="69" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A69" s="53"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="49"/>
+      <c r="D69" s="17"/>
+      <c r="E69"/>
+      <c r="F69" s="16"/>
+      <c r="G69" s="16"/>
+      <c r="H69"/>
+      <c r="I69" s="20"/>
+      <c r="J69" s="23"/>
+      <c r="K69" s="23"/>
+      <c r="L69" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M69" s="23"/>
+      <c r="N69" s="23"/>
+      <c r="O69" s="23"/>
+      <c r="P69" s="13"/>
+      <c r="Q69" s="13"/>
+      <c r="R69" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S69" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T69" s="2"/>
+      <c r="U69" s="2"/>
+      <c r="V69"/>
+      <c r="W69"/>
+    </row>
+    <row r="70" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A70" s="53"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="49"/>
+      <c r="D70" s="15"/>
+      <c r="E70"/>
+      <c r="F70" s="16"/>
+      <c r="G70" s="16"/>
+      <c r="H70"/>
+      <c r="I70" s="20"/>
+      <c r="J70" s="23"/>
+      <c r="K70" s="23"/>
+      <c r="L70" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="M70" s="23"/>
+      <c r="N70" s="23"/>
+      <c r="O70" s="23"/>
+      <c r="P70" s="13"/>
+      <c r="Q70" s="13"/>
+      <c r="R70" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S70" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T70" s="2"/>
+      <c r="U70" s="2"/>
+      <c r="V70"/>
+      <c r="W70"/>
+    </row>
+    <row r="71" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="53"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="49"/>
+      <c r="D71" s="15"/>
+      <c r="E71"/>
+      <c r="F71" s="16"/>
+      <c r="G71" s="16"/>
+      <c r="H71"/>
+      <c r="I71" s="10"/>
+      <c r="J71" s="21"/>
+      <c r="K71" s="21"/>
+      <c r="L71" s="23"/>
+      <c r="M71" s="21"/>
+      <c r="N71" s="21"/>
+      <c r="O71" s="21"/>
+      <c r="P71"/>
+      <c r="Q71"/>
+      <c r="R71" s="50" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S71" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T71" s="2"/>
+      <c r="U71" s="2"/>
+      <c r="V71"/>
+      <c r="W71"/>
+    </row>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A72" s="58"/>
+      <c r="B72" s="58"/>
+      <c r="C72" s="59"/>
+      <c r="D72" s="60"/>
+      <c r="E72" s="61"/>
+      <c r="F72" s="62"/>
+      <c r="G72" s="62"/>
+      <c r="H72" s="61"/>
+      <c r="I72" s="63"/>
+      <c r="J72" s="64"/>
+      <c r="K72" s="64"/>
+      <c r="L72" s="65"/>
+      <c r="M72" s="64"/>
+      <c r="N72" s="64"/>
+      <c r="O72" s="64"/>
+      <c r="P72" s="61"/>
+      <c r="Q72" s="61"/>
+      <c r="R72" s="61"/>
+      <c r="S72" s="39"/>
+      <c r="T72" s="38"/>
+      <c r="U72" s="38"/>
+      <c r="V72"/>
+      <c r="W72"/>
+    </row>
+    <row r="73" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A73" s="56" t="s">
+        <v>12</v>
+      </c>
+      <c r="B73" s="40"/>
+      <c r="C73" s="39"/>
+      <c r="D73" s="66"/>
+      <c r="E73" s="39"/>
+      <c r="F73" s="71"/>
+      <c r="G73" s="67"/>
+      <c r="H73" s="39"/>
+      <c r="I73" s="68"/>
+      <c r="J73" s="41"/>
+      <c r="K73" s="41"/>
+      <c r="L73" s="69" t="s">
+        <v>39</v>
+      </c>
+      <c r="M73" s="41"/>
+      <c r="N73" s="41"/>
+      <c r="O73" s="41"/>
+      <c r="P73" s="39"/>
+      <c r="Q73" s="39"/>
+      <c r="R73" s="70" t="s">
+        <v>39</v>
+      </c>
+      <c r="S73" s="70" t="s">
+        <v>39</v>
+      </c>
+      <c r="T73" s="38"/>
+      <c r="U73" s="38"/>
+      <c r="V73"/>
+      <c r="W73"/>
+    </row>
+    <row r="74" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A74" s="58"/>
+      <c r="B74" s="58"/>
+      <c r="C74" s="39"/>
+      <c r="D74" s="66"/>
+      <c r="E74" s="39"/>
+      <c r="F74" s="71"/>
+      <c r="G74" s="71"/>
+      <c r="H74" s="39"/>
+      <c r="I74" s="68"/>
+      <c r="J74" s="41"/>
+      <c r="K74" s="41"/>
+      <c r="L74" s="69" t="s">
+        <v>39</v>
+      </c>
+      <c r="M74" s="72"/>
+      <c r="N74" s="72"/>
+      <c r="O74" s="72"/>
+      <c r="P74" s="73"/>
+      <c r="Q74" s="73"/>
+      <c r="R74" s="70" t="s">
+        <v>39</v>
+      </c>
+      <c r="S74" s="70" t="s">
+        <v>39</v>
+      </c>
+      <c r="T74" s="38"/>
+      <c r="U74" s="38"/>
+      <c r="V74"/>
+      <c r="W74"/>
+    </row>
+    <row r="75" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A75" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="B75" s="40"/>
+      <c r="C75" s="39"/>
+      <c r="D75" s="74"/>
+      <c r="E75" s="39"/>
+      <c r="F75" s="71"/>
+      <c r="G75" s="71"/>
+      <c r="H75" s="39"/>
+      <c r="I75" s="68"/>
+      <c r="J75" s="41"/>
+      <c r="K75" s="41"/>
+      <c r="L75" s="78" t="s">
+        <v>40</v>
+      </c>
+      <c r="M75" s="78"/>
+      <c r="N75" s="78"/>
+      <c r="O75" s="78"/>
+      <c r="P75" s="78"/>
+      <c r="Q75" s="78"/>
+      <c r="R75" s="78"/>
+      <c r="S75" s="78"/>
+      <c r="T75" s="38"/>
+      <c r="U75" s="38"/>
+      <c r="V75"/>
+      <c r="W75"/>
+    </row>
+    <row r="76" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="D76" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E76" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F36" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G36" s="6" t="s">
+      <c r="F76" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G76" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H36" s="7"/>
-      <c r="I36" s="9" t="s">
+      <c r="H76" s="7"/>
+      <c r="I76" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="T36" s="25" t="s">
+      <c r="T76" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="U36" s="25" t="s">
+      <c r="U76" s="25" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.2"/>
-    <row r="49" x14ac:dyDescent="0.2"/>
-    <row r="50" x14ac:dyDescent="0.2"/>
-    <row r="51" x14ac:dyDescent="0.2"/>
-    <row r="52" x14ac:dyDescent="0.2"/>
-    <row r="53" x14ac:dyDescent="0.2"/>
-    <row r="54" x14ac:dyDescent="0.2"/>
-    <row r="55" x14ac:dyDescent="0.2"/>
-    <row r="56" x14ac:dyDescent="0.2"/>
-    <row r="57" x14ac:dyDescent="0.2"/>
-    <row r="58" x14ac:dyDescent="0.2"/>
-    <row r="59" x14ac:dyDescent="0.2"/>
-    <row r="60" x14ac:dyDescent="0.2"/>
-    <row r="61" x14ac:dyDescent="0.2"/>
-    <row r="62" x14ac:dyDescent="0.2"/>
-    <row r="63" x14ac:dyDescent="0.2"/>
-    <row r="64" x14ac:dyDescent="0.2"/>
-    <row r="65" x14ac:dyDescent="0.2"/>
-    <row r="66" x14ac:dyDescent="0.2"/>
-    <row r="67" x14ac:dyDescent="0.2"/>
-    <row r="68" x14ac:dyDescent="0.2"/>
-    <row r="69" x14ac:dyDescent="0.2"/>
-    <row r="70" x14ac:dyDescent="0.2"/>
-    <row r="71" x14ac:dyDescent="0.2"/>
-    <row r="72" x14ac:dyDescent="0.2"/>
-    <row r="73" x14ac:dyDescent="0.2"/>
-    <row r="74" x14ac:dyDescent="0.2"/>
-    <row r="75" x14ac:dyDescent="0.2"/>
-    <row r="76" x14ac:dyDescent="0.2"/>
-    <row r="77" x14ac:dyDescent="0.2"/>
-    <row r="78" x14ac:dyDescent="0.2"/>
-    <row r="79" x14ac:dyDescent="0.2"/>
-    <row r="80" x14ac:dyDescent="0.2"/>
+    <row r="77" spans="1:23" x14ac:dyDescent="0.2"/>
+    <row r="78" spans="1:23" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="1:23" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="1:23" x14ac:dyDescent="0.2"/>
     <row r="81" x14ac:dyDescent="0.2"/>
     <row r="82" x14ac:dyDescent="0.2"/>
     <row r="83" x14ac:dyDescent="0.2"/>
@@ -2762,12 +4078,54 @@
     <row r="250" x14ac:dyDescent="0.2"/>
     <row r="251" x14ac:dyDescent="0.2"/>
     <row r="252" x14ac:dyDescent="0.2"/>
+    <row r="253" x14ac:dyDescent="0.2"/>
+    <row r="254" x14ac:dyDescent="0.2"/>
+    <row r="255" x14ac:dyDescent="0.2"/>
+    <row r="256" x14ac:dyDescent="0.2"/>
+    <row r="257" x14ac:dyDescent="0.2"/>
+    <row r="258" x14ac:dyDescent="0.2"/>
+    <row r="259" x14ac:dyDescent="0.2"/>
+    <row r="260" x14ac:dyDescent="0.2"/>
+    <row r="261" x14ac:dyDescent="0.2"/>
+    <row r="262" x14ac:dyDescent="0.2"/>
+    <row r="263" x14ac:dyDescent="0.2"/>
+    <row r="264" x14ac:dyDescent="0.2"/>
+    <row r="265" x14ac:dyDescent="0.2"/>
+    <row r="266" x14ac:dyDescent="0.2"/>
+    <row r="267" x14ac:dyDescent="0.2"/>
+    <row r="268" x14ac:dyDescent="0.2"/>
+    <row r="269" x14ac:dyDescent="0.2"/>
+    <row r="270" x14ac:dyDescent="0.2"/>
+    <row r="271" x14ac:dyDescent="0.2"/>
+    <row r="272" x14ac:dyDescent="0.2"/>
+    <row r="273" x14ac:dyDescent="0.2"/>
+    <row r="274" x14ac:dyDescent="0.2"/>
+    <row r="275" x14ac:dyDescent="0.2"/>
+    <row r="276" x14ac:dyDescent="0.2"/>
+    <row r="277" x14ac:dyDescent="0.2"/>
+    <row r="278" x14ac:dyDescent="0.2"/>
+    <row r="279" x14ac:dyDescent="0.2"/>
+    <row r="280" x14ac:dyDescent="0.2"/>
+    <row r="281" x14ac:dyDescent="0.2"/>
+    <row r="282" x14ac:dyDescent="0.2"/>
+    <row r="283" x14ac:dyDescent="0.2"/>
+    <row r="284" x14ac:dyDescent="0.2"/>
+    <row r="285" x14ac:dyDescent="0.2"/>
+    <row r="286" x14ac:dyDescent="0.2"/>
+    <row r="287" x14ac:dyDescent="0.2"/>
+    <row r="288" x14ac:dyDescent="0.2"/>
+    <row r="289" x14ac:dyDescent="0.2"/>
+    <row r="290" x14ac:dyDescent="0.2"/>
+    <row r="291" x14ac:dyDescent="0.2"/>
+    <row r="292" x14ac:dyDescent="0.2"/>
+    <row r="293" x14ac:dyDescent="0.2"/>
+    <row r="294" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:U31">
-    <sortCondition descending="1" ref="S8:S31"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:S71">
+    <sortCondition descending="1" ref="S8:S71"/>
   </sortState>
   <mergeCells count="9">
-    <mergeCell ref="L35:S35"/>
+    <mergeCell ref="L75:S75"/>
     <mergeCell ref="M5:R5"/>
     <mergeCell ref="C4:R4"/>
     <mergeCell ref="M6:N6"/>
@@ -2778,11 +4136,11 @@
     <mergeCell ref="S5:U5"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <conditionalFormatting sqref="S8:S31">
-    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="lessThan">
+  <conditionalFormatting sqref="S8:S71">
+    <cfRule type="cellIs" dxfId="1" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.35433070866141736" right="0.39370078740157483" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" scale="89" fitToHeight="10" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>